<commit_message>
Lots of changes.... Norm RMSE to median
</commit_message>
<xml_diff>
--- a/inputs/SUBParameters.xlsx
+++ b/inputs/SUBParameters.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtsoonthornran\Downloads\Publications\1stPaper\CodeFig\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtsoonthornran\BKKSubPastasModels\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DDDED4-ABBC-40CF-9E6D-E4386650142A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="K" sheetId="21" r:id="rId1"/>
@@ -17,10 +18,21 @@
     <sheet name="Sskv" sheetId="18" r:id="rId3"/>
     <sheet name="Sske" sheetId="19" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -149,7 +161,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -185,20 +197,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -479,10 +487,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
@@ -495,28 +503,28 @@
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1159,7 +1167,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B24" s="1">
@@ -1188,7 +1196,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="1">
@@ -1217,7 +1225,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B26" s="1">
@@ -1246,7 +1254,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B27" s="1">
@@ -1275,7 +1283,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B28" s="1">
@@ -1304,7 +1312,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="1">
@@ -1333,7 +1341,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="1">
@@ -1362,7 +1370,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="1">
@@ -1397,7 +1405,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1419,13 +1427,13 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -2075,7 +2083,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B24">
@@ -2104,7 +2112,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B25">
@@ -2133,7 +2141,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B26">
@@ -2162,7 +2170,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B27">
@@ -2191,7 +2199,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B28">
@@ -2225,7 +2233,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2248,28 +2256,28 @@
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="K1" s="2"/>
@@ -2278,28 +2286,28 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="5">
         <v>9.8044527099084341E-4</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="5">
         <v>9.548379662498979E-5</v>
       </c>
       <c r="D2" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="5">
         <v>9.2270199652400904E-5</v>
       </c>
       <c r="F2" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="5">
         <v>8.8670877910996222E-5</v>
       </c>
       <c r="H2" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="5">
         <v>4.8506542485757792E-5</v>
       </c>
     </row>
@@ -2307,28 +2315,28 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <v>4.9484652182067376E-4</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <v>4.8572133008237997E-5</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="5">
         <v>4.7741898312494817E-4</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <v>4.6587219190804714E-5</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="5">
         <v>4.5633977302917989E-4</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="5">
         <v>4.4941205889230356E-5</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="5">
         <v>4.4420475576615557E-4</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="5">
         <v>2.4253271242878896E-5</v>
       </c>
     </row>
@@ -2336,28 +2344,28 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>2.4801111994161061E-3</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <v>2.426758003487599E-4</v>
       </c>
       <c r="D4" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <v>2.3179765218107521E-4</v>
       </c>
       <c r="F4" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="5">
         <v>2.2139509860204666E-4</v>
       </c>
       <c r="H4" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="5">
         <v>1.2126635621439448E-4</v>
       </c>
     </row>
@@ -2365,28 +2373,28 @@
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>2.4683939166376461E-3</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>2.4175756035617484E-4</v>
       </c>
       <c r="D5" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <v>2.3131475535011746E-4</v>
       </c>
       <c r="F5" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="5">
         <v>2.2167719477749056E-4</v>
       </c>
       <c r="H5" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="5">
         <v>1.2126635621439448E-4</v>
       </c>
     </row>
@@ -2394,28 +2402,28 @@
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="5">
         <v>7.428563057470354E-3</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <v>7.2363430458604477E-4</v>
       </c>
       <c r="D6" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>6.9202649739300676E-4</v>
       </c>
       <c r="F6" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="5">
         <v>6.6041682225121106E-4</v>
       </c>
       <c r="H6" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="5">
         <v>3.6379906864318341E-4</v>
       </c>
     </row>
@@ -2423,28 +2431,28 @@
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="5">
         <v>1.2312973571959758E-3</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <v>1.2069653912651356E-4</v>
       </c>
       <c r="D7" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
         <v>1.1663220402473934E-4</v>
       </c>
       <c r="F7" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="5">
         <v>1.1235301472307589E-4</v>
       </c>
       <c r="H7" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="5">
         <v>6.0633178107197238E-5</v>
       </c>
     </row>
@@ -2452,28 +2460,28 @@
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="5">
         <v>3.9587721745653901E-3</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="5">
         <v>3.8335094292073939E-4</v>
       </c>
       <c r="D8" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <v>3.6311529104932668E-4</v>
       </c>
       <c r="F8" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="5">
         <v>3.515599741109437E-4</v>
       </c>
       <c r="H8" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="5">
         <v>1.9402616994303117E-4</v>
       </c>
     </row>
@@ -2481,28 +2489,28 @@
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="5">
         <v>8.0000000000000019E-3</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="5">
         <v>7.9935696583604632E-4</v>
       </c>
       <c r="D9" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <v>7.0356066459320056E-4</v>
       </c>
       <c r="F9" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="5">
         <v>6.596147590416816E-4</v>
       </c>
       <c r="H9" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="5">
         <v>3.8805233988606233E-4</v>
       </c>
     </row>
@@ -2510,28 +2518,28 @@
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="5">
         <v>1.9700757715135613E-3</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="5">
         <v>1.9124982829123489E-4</v>
       </c>
       <c r="D10" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="5">
         <v>1.8454039930480181E-4</v>
       </c>
       <c r="F10" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="5">
         <v>1.7883006891226079E-4</v>
       </c>
       <c r="H10" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="5">
         <v>9.7013084971515583E-5</v>
       </c>
     </row>
@@ -2539,28 +2547,28 @@
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <v>3.4530390739466979E-3</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="5">
         <v>3.3846058449864475E-4</v>
       </c>
       <c r="D11" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="5">
         <v>3.2294569878340315E-4</v>
       </c>
       <c r="F11" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="5">
         <v>3.1174237933433992E-4</v>
       </c>
       <c r="H11" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="5">
         <v>1.6977289870015227E-4</v>
       </c>
     </row>
@@ -2568,28 +2576,28 @@
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="5">
         <v>2.4761876858234513E-3</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="5">
         <v>2.4121143486201491E-4</v>
       </c>
       <c r="D12" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="5">
         <v>2.3067549913100227E-4</v>
       </c>
       <c r="F12" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="5">
         <v>2.201389407504037E-4</v>
       </c>
       <c r="H12" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="5">
         <v>1.2126635621439448E-4</v>
       </c>
     </row>
@@ -2597,28 +2605,28 @@
       <c r="A13" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <v>1.979386087282695E-3</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="5">
         <v>1.9428853203295199E-4</v>
       </c>
       <c r="D13" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="5">
         <v>1.8687527039520658E-4</v>
       </c>
       <c r="F13" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="5">
         <v>1.8253590921167207E-4</v>
       </c>
       <c r="H13" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="5">
         <v>9.7013084971515583E-5</v>
       </c>
     </row>
@@ -2626,28 +2634,28 @@
       <c r="A14" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="5">
         <v>2.4742326091033688E-4</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="5">
         <v>2.4230729170731099E-5</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="5">
         <v>2.3888569840924834E-4</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="5">
         <v>2.337594436110171E-5</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="5">
         <v>2.277090285662372E-4</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="5">
         <v>2.2426571966825683E-5</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="5">
         <v>2.2196037727514658E-4</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="5">
         <v>1.2126635621439448E-5</v>
       </c>
     </row>
@@ -2655,28 +2663,28 @@
       <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="5">
         <v>1.7333313800764159E-3</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="5">
         <v>1.703924018756886E-4</v>
       </c>
       <c r="D15" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="5">
         <v>1.6091861830274718E-4</v>
       </c>
       <c r="F15" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="5">
         <v>1.5380748867353786E-4</v>
       </c>
       <c r="H15" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="5">
         <v>8.4886449350076137E-5</v>
       </c>
     </row>
@@ -2684,28 +2692,28 @@
       <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="5">
         <v>2.9808631547078423E-3</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="5">
         <v>2.9277418149203417E-4</v>
       </c>
       <c r="D16" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="5">
         <v>2.7719336713683305E-4</v>
       </c>
       <c r="F16" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="5">
         <v>2.6268490885423374E-4</v>
       </c>
       <c r="H16" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="5">
         <v>1.4551962745727338E-4</v>
       </c>
     </row>
@@ -2713,28 +2721,28 @@
       <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="5">
         <v>4.9445639308626655E-4</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="5">
         <v>4.8535160069751977E-5</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="5">
         <v>4.7777139681849667E-4</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="5">
         <v>4.6685815300294451E-5</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="5">
         <v>4.5664824786201713E-4</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="5">
         <v>4.4970675219604504E-5</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="5">
         <v>4.4506005352310294E-4</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="5">
         <v>2.4253271242878896E-5</v>
       </c>
     </row>
@@ -2742,28 +2750,28 @@
       <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="5">
         <v>3.714281528735177E-3</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="5">
         <v>3.6346093756096649E-4</v>
       </c>
       <c r="D18" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="5">
         <v>3.5238999064130536E-4</v>
       </c>
       <c r="F18" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="5">
         <v>3.4769647827161278E-4</v>
       </c>
       <c r="H18" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="5">
         <v>1.8189953432159171E-4</v>
       </c>
     </row>
@@ -2771,28 +2779,28 @@
       <c r="A19" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="5">
         <v>9.8426814116861863E-4</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="5">
         <v>9.6630047857710865E-5</v>
       </c>
       <c r="D19" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="5">
         <v>9.4308381424504671E-5</v>
       </c>
       <c r="F19" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="5">
         <v>9.1206383510351521E-5</v>
       </c>
       <c r="H19" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="5">
         <v>4.8506542485757792E-5</v>
       </c>
     </row>
@@ -2800,28 +2808,28 @@
       <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="5">
         <v>7.4226978273101069E-4</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="5">
         <v>7.2802740104627959E-5</v>
       </c>
       <c r="D20" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="5">
         <v>6.9394426605035226E-5</v>
       </c>
       <c r="F20" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="5">
         <v>6.7148396165000207E-5</v>
       </c>
       <c r="H20" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="5">
         <v>3.6379906864318345E-5</v>
       </c>
     </row>
@@ -2829,28 +2837,28 @@
       <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="5">
         <v>4.9602223988322119E-4</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="5">
         <v>4.8535160069751977E-5</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="5">
         <v>4.7566823169218855E-4</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="5">
         <v>4.635953043621504E-5</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="5">
         <v>4.5268585116385211E-4</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="5">
         <v>4.4279019720409334E-5</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="5">
         <v>4.3325564085736328E-4</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="5">
         <v>2.4253271242878896E-5</v>
       </c>
     </row>
@@ -2858,28 +2866,28 @@
       <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="5">
         <v>4.9602223988322123E-3</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="5">
         <v>4.853516006975198E-4</v>
       </c>
       <c r="D22" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="5">
         <v>4.6359530436215041E-4</v>
       </c>
       <c r="F22" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="5">
         <v>4.4279019720409331E-4</v>
       </c>
       <c r="H22" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="5">
         <v>2.4253271242878895E-4</v>
       </c>
     </row>
@@ -2887,268 +2895,268 @@
       <c r="A23" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="5">
         <v>1.9840889595328847E-3</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="5">
         <v>1.9414064027900791E-4</v>
       </c>
       <c r="D23" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="5">
         <v>1.8543812174486016E-4</v>
       </c>
       <c r="F23" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="5">
         <v>1.7711607888163734E-4</v>
       </c>
       <c r="H23" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="5">
         <v>9.7013084971515583E-5</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="5">
         <v>2.4761876858234513E-4</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="5">
         <v>2.4341771696526945E-5</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="5">
         <v>2.3906228536404344E-4</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="5">
         <v>2.3543216837781408E-5</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="5">
         <v>2.334290765014721E-4</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="5">
         <v>2.2832412393100853E-5</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="5">
         <v>2.2210237788307778E-4</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="5">
         <v>1.2126635621439448E-5</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="5">
         <v>9.9125888433051895E-3</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="5">
         <v>9.6776160685979259E-4</v>
       </c>
       <c r="D25" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="5">
         <v>9.3437635197603295E-4</v>
       </c>
       <c r="F25" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="5">
         <v>9.0961330323741367E-4</v>
       </c>
       <c r="H25" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="5">
         <v>4.850654248575779E-4</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="5">
         <v>5.0000000000000012E-4</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="5">
         <v>5.0000000000000043E-5</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="5">
         <v>5.0000000000000012E-4</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="5">
         <v>5.0000000000000043E-5</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="5">
         <v>5.0000000000000012E-4</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="5">
         <v>5.0000000000000043E-5</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="5">
         <v>5.0000000000000012E-4</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I26" s="5">
         <v>5.0000000000000043E-5</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="5">
         <v>5.0000000000000012E-4</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="5">
         <v>5.0000000000000043E-5</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="5">
         <v>5.0000000000000012E-4</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="5">
         <v>5.0000000000000043E-5</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="5">
         <v>5.0000000000000012E-4</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="5">
         <v>5.0000000000000043E-5</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27" s="5">
         <v>5.0000000000000012E-4</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="5">
         <v>5.0000000000000043E-5</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="5">
         <v>5.0000000000000012E-4</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="5">
         <v>5.0000000000000043E-5</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="5">
         <v>5.0000000000000012E-4</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="5">
         <v>5.0000000000000043E-5</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="5">
         <v>5.0000000000000012E-4</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="5">
         <v>5.0000000000000043E-5</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="5">
         <v>5.0000000000000012E-4</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="5">
         <v>5.0000000000000043E-5</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="5">
         <v>5.0000000000000012E-4</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="5">
         <v>4.9959810364752895E-5</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="5">
         <v>4.7706732717378721E-4</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="5">
         <v>4.3972541537075035E-5</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="5">
         <v>4.2162645838521675E-4</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="5">
         <v>4.12259224401051E-5</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H29" s="5">
         <v>4.1023928592577352E-4</v>
       </c>
-      <c r="I29" s="7">
+      <c r="I29" s="5">
         <v>2.4253271242878896E-5</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="5">
         <v>1.2265080218123586E-3</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="5">
         <v>1.2024440754700463E-4</v>
       </c>
       <c r="D30" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="5">
         <v>1.1324675411436813E-4</v>
       </c>
       <c r="F30" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="5">
         <v>1.1000034653859286E-4</v>
       </c>
       <c r="H30" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I30" s="7">
+      <c r="I30" s="5">
         <v>6.0633178107197238E-5</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="5">
         <v>1.2380938429117257E-3</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="5">
         <v>1.2078755982213858E-4</v>
       </c>
       <c r="D31" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="5">
         <v>1.1606062195794044E-4</v>
       </c>
       <c r="F31" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="5">
         <v>1.1370166290467671E-4</v>
       </c>
       <c r="H31" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
-      <c r="I31" s="7">
+      <c r="I31" s="5">
         <v>6.0633178107197238E-5</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="4"/>
+      <c r="A33" s="3"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="4"/>
+      <c r="A34" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3157,11 +3165,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3173,28 +3181,28 @@
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3206,25 +3214,29 @@
         <v>7.3533395324313258E-5</v>
       </c>
       <c r="C2" s="1">
-        <v>7.1612847468742353E-6</v>
+        <f>B2/10</f>
+        <v>7.3533395324313255E-6</v>
       </c>
       <c r="D2" s="1">
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="E2" s="1">
-        <v>6.9202649739300671E-6</v>
+        <f>D2/10</f>
+        <v>4.0000000000000007E-6</v>
       </c>
       <c r="F2" s="1">
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="G2" s="1">
-        <v>6.6503158433247165E-6</v>
+        <f>F2/10</f>
+        <v>1.5000000000000002E-6</v>
       </c>
       <c r="H2" s="1">
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="I2" s="1">
-        <v>3.6379906864318344E-6</v>
+        <f>H2/10</f>
+        <v>1.5000000000000002E-6</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -3235,25 +3247,29 @@
         <v>1.2371163045516843E-5</v>
       </c>
       <c r="C3" s="1">
-        <v>1.21430332520595E-6</v>
+        <f t="shared" ref="C3:E31" si="0">B3/10</f>
+        <v>1.2371163045516842E-6</v>
       </c>
       <c r="D3" s="1">
         <v>1.1935474578123703E-5</v>
       </c>
       <c r="E3" s="1">
-        <v>1.1646804797701178E-6</v>
+        <f t="shared" ref="E3" si="1">D3/10</f>
+        <v>1.1935474578123704E-6</v>
       </c>
       <c r="F3" s="1">
         <v>1.1408494325729498E-5</v>
       </c>
       <c r="G3" s="1">
-        <v>1.123530147230759E-6</v>
+        <f t="shared" ref="G3" si="2">F3/10</f>
+        <v>1.1408494325729497E-6</v>
       </c>
       <c r="H3" s="1">
         <v>1.1105118894153889E-5</v>
       </c>
       <c r="I3" s="1">
-        <v>6.063317810719724E-7</v>
+        <f t="shared" ref="I3" si="3">H3/10</f>
+        <v>1.1105118894153888E-6</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -3264,25 +3280,29 @@
         <v>2.4801111994161059E-4</v>
       </c>
       <c r="C4" s="1">
-        <v>2.4267580034875989E-5</v>
+        <f t="shared" si="0"/>
+        <v>2.4801111994161058E-5</v>
       </c>
       <c r="D4" s="1">
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="E4" s="1">
-        <v>2.317976521810752E-5</v>
+        <f t="shared" ref="E4" si="4">D4/10</f>
+        <v>4.0000000000000007E-6</v>
       </c>
       <c r="F4" s="1">
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="G4" s="1">
-        <v>2.2139509860204667E-5</v>
+        <f t="shared" ref="G4" si="5">F4/10</f>
+        <v>1.5000000000000002E-6</v>
       </c>
       <c r="H4" s="1">
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="I4" s="1">
-        <v>1.2126635621439448E-5</v>
+        <f t="shared" ref="I4" si="6">H4/10</f>
+        <v>1.5000000000000002E-6</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -3293,25 +3313,29 @@
         <v>2.4683939166376463E-4</v>
       </c>
       <c r="C5" s="1">
-        <v>2.4175756035617484E-5</v>
+        <f t="shared" si="0"/>
+        <v>2.4683939166376464E-5</v>
       </c>
       <c r="D5" s="1">
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="E5" s="1">
-        <v>2.3131475535011744E-5</v>
+        <f t="shared" ref="E5" si="7">D5/10</f>
+        <v>4.0000000000000007E-6</v>
       </c>
       <c r="F5" s="1">
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="G5" s="1">
-        <v>2.2167719477749056E-5</v>
+        <f t="shared" ref="G5" si="8">F5/10</f>
+        <v>1.5000000000000002E-6</v>
       </c>
       <c r="H5" s="1">
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="I5" s="1">
-        <v>1.2126635621439448E-5</v>
+        <f t="shared" ref="I5" si="9">H5/10</f>
+        <v>1.5000000000000002E-6</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -3322,25 +3346,29 @@
         <v>1.0895225817623185E-4</v>
       </c>
       <c r="C6" s="1">
-        <v>1.0613303133928656E-5</v>
+        <f t="shared" si="0"/>
+        <v>1.0895225817623186E-5</v>
       </c>
       <c r="D6" s="1">
         <v>7.9999999999999996E-6</v>
       </c>
       <c r="E6" s="1">
-        <v>1.01497219617641E-5</v>
+        <f t="shared" ref="E6" si="10">D6/10</f>
+        <v>7.9999999999999996E-7</v>
       </c>
       <c r="F6" s="1">
         <v>3.0000000000000001E-6</v>
       </c>
       <c r="G6" s="1">
-        <v>9.6861133930177624E-6</v>
+        <f t="shared" ref="G6" si="11">F6/10</f>
+        <v>2.9999999999999999E-7</v>
       </c>
       <c r="H6" s="1">
         <v>3.0000000000000001E-6</v>
       </c>
       <c r="I6" s="1">
-        <v>5.3357196734333566E-6</v>
+        <f t="shared" ref="I6" si="12">H6/10</f>
+        <v>2.9999999999999999E-7</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -3351,25 +3379,29 @@
         <v>1.2312973571959758E-4</v>
       </c>
       <c r="C7" s="1">
-        <v>1.2069653912651355E-5</v>
+        <f t="shared" si="0"/>
+        <v>1.2312973571959758E-5</v>
       </c>
       <c r="D7" s="1">
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="E7" s="1">
-        <v>1.1663220402473934E-5</v>
+        <f t="shared" ref="E7" si="13">D7/10</f>
+        <v>4.0000000000000007E-6</v>
       </c>
       <c r="F7" s="1">
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="G7" s="1">
-        <v>1.1235301472307589E-5</v>
+        <f t="shared" ref="G7" si="14">F7/10</f>
+        <v>1.5000000000000002E-6</v>
       </c>
       <c r="H7" s="1">
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="I7" s="1">
-        <v>6.063317810719724E-6</v>
+        <f t="shared" ref="I7" si="15">H7/10</f>
+        <v>1.5000000000000002E-6</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -3380,25 +3412,29 @@
         <v>3.9587721745653903E-5</v>
       </c>
       <c r="C8" s="1">
-        <v>3.8335094292073943E-6</v>
+        <f t="shared" si="0"/>
+        <v>3.9587721745653904E-6</v>
       </c>
       <c r="D8" s="1">
         <v>7.9999999999999996E-6</v>
       </c>
       <c r="E8" s="1">
-        <v>3.6311529104932668E-6</v>
+        <f t="shared" ref="E8" si="16">D8/10</f>
+        <v>7.9999999999999996E-7</v>
       </c>
       <c r="F8" s="1">
         <v>3.0000000000000001E-6</v>
       </c>
       <c r="G8" s="1">
-        <v>3.5155997411094372E-6</v>
+        <f t="shared" ref="G8" si="17">F8/10</f>
+        <v>2.9999999999999999E-7</v>
       </c>
       <c r="H8" s="1">
         <v>3.0000000000000001E-6</v>
       </c>
       <c r="I8" s="1">
-        <v>1.9402616994303117E-6</v>
+        <f t="shared" ref="I8" si="18">H8/10</f>
+        <v>2.9999999999999999E-7</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -3409,25 +3445,29 @@
         <v>5.3333333333333347E-5</v>
       </c>
       <c r="C9" s="1">
-        <v>5.3290464389069752E-6</v>
+        <f t="shared" si="0"/>
+        <v>5.3333333333333345E-6</v>
       </c>
       <c r="D9" s="1">
         <v>5.3333333333333337E-6</v>
       </c>
       <c r="E9" s="1">
-        <v>4.690404430621337E-6</v>
+        <f t="shared" ref="E9" si="19">D9/10</f>
+        <v>5.3333333333333334E-7</v>
       </c>
       <c r="F9" s="1">
         <v>2.0000000000000003E-6</v>
       </c>
       <c r="G9" s="1">
-        <v>4.3974317269445439E-6</v>
+        <f t="shared" ref="G9" si="20">F9/10</f>
+        <v>2.0000000000000004E-7</v>
       </c>
       <c r="H9" s="1">
         <v>2.0000000000000003E-6</v>
       </c>
       <c r="I9" s="1">
-        <v>2.5870155992404154E-6</v>
+        <f t="shared" ref="I9" si="21">H9/10</f>
+        <v>2.0000000000000004E-7</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -3438,25 +3478,29 @@
         <v>1.9700757715135613E-4</v>
       </c>
       <c r="C10" s="1">
-        <v>1.9124982829123487E-5</v>
+        <f t="shared" si="0"/>
+        <v>1.9700757715135615E-5</v>
       </c>
       <c r="D10" s="1">
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="E10" s="1">
-        <v>1.845403993048018E-5</v>
+        <f t="shared" ref="E10" si="22">D10/10</f>
+        <v>4.0000000000000007E-6</v>
       </c>
       <c r="F10" s="1">
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="G10" s="1">
-        <v>1.7883006891226079E-5</v>
+        <f t="shared" ref="G10" si="23">F10/10</f>
+        <v>1.5000000000000002E-6</v>
       </c>
       <c r="H10" s="1">
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="I10" s="1">
-        <v>9.7013084971515583E-6</v>
+        <f t="shared" ref="I10" si="24">H10/10</f>
+        <v>1.5000000000000002E-6</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -3467,25 +3511,29 @@
         <v>2.4664564813904984E-4</v>
       </c>
       <c r="C11" s="1">
-        <v>2.4175756035617484E-5</v>
+        <f t="shared" si="0"/>
+        <v>2.4664564813904983E-5</v>
       </c>
       <c r="D11" s="1">
         <v>2.6666666666666667E-5</v>
       </c>
       <c r="E11" s="1">
-        <v>2.3067549913100226E-5</v>
+        <f t="shared" ref="E11" si="25">D11/10</f>
+        <v>2.6666666666666668E-6</v>
       </c>
       <c r="F11" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="G11" s="1">
-        <v>2.2267312809595709E-5</v>
+        <f t="shared" ref="G11" si="26">F11/10</f>
+        <v>1.0000000000000002E-6</v>
       </c>
       <c r="H11" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="I11" s="1">
-        <v>1.2126635621439448E-5</v>
+        <f t="shared" ref="I11" si="27">H11/10</f>
+        <v>1.0000000000000002E-6</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -3496,25 +3544,29 @@
         <v>1.2380938429117257E-4</v>
       </c>
       <c r="C12" s="1">
-        <v>1.2060571743100746E-5</v>
+        <f t="shared" si="0"/>
+        <v>1.2380938429117256E-5</v>
       </c>
       <c r="D12" s="1">
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="E12" s="1">
-        <v>1.1533774956550113E-5</v>
+        <f t="shared" ref="E12" si="28">D12/10</f>
+        <v>2.0000000000000003E-6</v>
       </c>
       <c r="F12" s="1">
         <v>7.500000000000001E-6</v>
       </c>
       <c r="G12" s="1">
-        <v>1.1006947037520185E-5</v>
+        <f t="shared" ref="G12" si="29">F12/10</f>
+        <v>7.5000000000000012E-7</v>
       </c>
       <c r="H12" s="1">
         <v>7.500000000000001E-6</v>
       </c>
       <c r="I12" s="1">
-        <v>6.063317810719724E-6</v>
+        <f t="shared" ref="I12" si="30">H12/10</f>
+        <v>7.5000000000000012E-7</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -3525,25 +3577,29 @@
         <v>1.9793860872826951E-5</v>
       </c>
       <c r="C13" s="1">
-        <v>1.9428853203295197E-6</v>
+        <f t="shared" si="0"/>
+        <v>1.9793860872826952E-6</v>
       </c>
       <c r="D13" s="1">
         <v>7.9999999999999996E-6</v>
       </c>
       <c r="E13" s="1">
-        <v>1.8687527039520657E-6</v>
+        <f t="shared" ref="E13" si="31">D13/10</f>
+        <v>7.9999999999999996E-7</v>
       </c>
       <c r="F13" s="1">
         <v>3.0000000000000001E-6</v>
       </c>
       <c r="G13" s="1">
-        <v>1.8253590921167207E-6</v>
+        <f t="shared" ref="G13" si="32">F13/10</f>
+        <v>2.9999999999999999E-7</v>
       </c>
       <c r="H13" s="1">
         <v>3.0000000000000001E-6</v>
       </c>
       <c r="I13" s="1">
-        <v>9.7013084971515587E-7</v>
+        <f t="shared" ref="I13" si="33">H13/10</f>
+        <v>2.9999999999999999E-7</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -3554,25 +3610,29 @@
         <v>2.4742326091033689E-6</v>
       </c>
       <c r="C14" s="1">
-        <v>2.4230729170731097E-7</v>
+        <f t="shared" si="0"/>
+        <v>2.474232609103369E-7</v>
       </c>
       <c r="D14" s="1">
         <v>2.3888569840924832E-6</v>
       </c>
       <c r="E14" s="1">
-        <v>2.337594436110171E-7</v>
+        <f t="shared" ref="E14" si="34">D14/10</f>
+        <v>2.3888569840924831E-7</v>
       </c>
       <c r="F14" s="1">
         <v>2.2770902856623721E-6</v>
       </c>
       <c r="G14" s="1">
-        <v>2.2426571966825684E-7</v>
+        <f t="shared" ref="G14" si="35">F14/10</f>
+        <v>2.2770902856623722E-7</v>
       </c>
       <c r="H14" s="1">
         <v>2.2196037727514661E-6</v>
       </c>
       <c r="I14" s="1">
-        <v>1.2126635621439448E-7</v>
+        <f t="shared" ref="I14" si="36">H14/10</f>
+        <v>2.2196037727514661E-7</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -3583,25 +3643,29 @@
         <v>8.6666569003820799E-5</v>
       </c>
       <c r="C15" s="1">
-        <v>8.5196200937844301E-6</v>
+        <f t="shared" si="0"/>
+        <v>8.6666569003820799E-6</v>
       </c>
       <c r="D15" s="1">
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="E15" s="1">
-        <v>8.0459309151373599E-6</v>
+        <f t="shared" ref="E15" si="37">D15/10</f>
+        <v>2.0000000000000003E-6</v>
       </c>
       <c r="F15" s="1">
         <v>7.500000000000001E-6</v>
       </c>
       <c r="G15" s="1">
-        <v>7.6903744336768937E-6</v>
+        <f t="shared" ref="G15" si="38">F15/10</f>
+        <v>7.5000000000000012E-7</v>
       </c>
       <c r="H15" s="1">
         <v>7.500000000000001E-6</v>
       </c>
       <c r="I15" s="1">
-        <v>4.2443224675038072E-6</v>
+        <f t="shared" ref="I15" si="39">H15/10</f>
+        <v>7.5000000000000012E-7</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -3612,28 +3676,32 @@
         <v>1.4904315773539212E-4</v>
       </c>
       <c r="C16" s="1">
-        <v>1.4638709074601709E-5</v>
+        <f t="shared" si="0"/>
+        <v>1.4904315773539212E-5</v>
       </c>
       <c r="D16" s="1">
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="E16" s="1">
-        <v>1.3859668356841653E-5</v>
+        <f t="shared" ref="E16" si="40">D16/10</f>
+        <v>2.0000000000000003E-6</v>
       </c>
       <c r="F16" s="1">
         <v>7.500000000000001E-6</v>
       </c>
       <c r="G16" s="1">
-        <v>1.3134245442711687E-5</v>
+        <f t="shared" ref="G16" si="41">F16/10</f>
+        <v>7.5000000000000012E-7</v>
       </c>
       <c r="H16" s="1">
         <v>7.500000000000001E-6</v>
       </c>
       <c r="I16" s="1">
-        <v>7.2759813728636687E-6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+        <f t="shared" ref="I16" si="42">H16/10</f>
+        <v>7.5000000000000012E-7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -3641,28 +3709,32 @@
         <v>1.2361409827156663E-5</v>
       </c>
       <c r="C17" s="1">
-        <v>1.2133790017437994E-6</v>
+        <f t="shared" si="0"/>
+        <v>1.2361409827156663E-6</v>
       </c>
       <c r="D17" s="1">
         <v>1.1944284920462416E-5</v>
       </c>
       <c r="E17" s="1">
-        <v>1.1671453825073612E-6</v>
+        <f t="shared" ref="E17" si="43">D17/10</f>
+        <v>1.1944284920462416E-6</v>
       </c>
       <c r="F17" s="1">
         <v>1.1416206196550428E-5</v>
       </c>
       <c r="G17" s="1">
-        <v>1.1242668804901126E-6</v>
+        <f t="shared" ref="G17" si="44">F17/10</f>
+        <v>1.1416206196550429E-6</v>
       </c>
       <c r="H17" s="1">
         <v>1.1126501338077573E-5</v>
       </c>
       <c r="I17" s="1">
-        <v>6.063317810719724E-7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+        <f t="shared" ref="I17" si="45">H17/10</f>
+        <v>1.1126501338077573E-6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -3670,28 +3742,32 @@
         <v>1.8571407643675885E-4</v>
       </c>
       <c r="C18" s="1">
-        <v>1.8173046878048325E-5</v>
+        <f t="shared" si="0"/>
+        <v>1.8571407643675884E-5</v>
       </c>
       <c r="D18" s="1">
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="E18" s="1">
-        <v>1.7619499532065267E-5</v>
+        <f t="shared" ref="E18" si="46">D18/10</f>
+        <v>2.0000000000000003E-6</v>
       </c>
       <c r="F18" s="1">
         <v>7.500000000000001E-6</v>
       </c>
       <c r="G18" s="1">
-        <v>1.7384823913580639E-5</v>
+        <f t="shared" ref="G18" si="47">F18/10</f>
+        <v>7.5000000000000012E-7</v>
       </c>
       <c r="H18" s="1">
         <v>7.500000000000001E-6</v>
       </c>
       <c r="I18" s="1">
-        <v>9.0949767160795847E-6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+        <f t="shared" ref="I18" si="48">H18/10</f>
+        <v>7.5000000000000012E-7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -3699,28 +3775,32 @@
         <v>9.8426814116861865E-5</v>
       </c>
       <c r="C19" s="1">
-        <v>9.6630047857710858E-6</v>
+        <f t="shared" si="0"/>
+        <v>9.8426814116861859E-6</v>
       </c>
       <c r="D19" s="1">
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="E19" s="1">
-        <v>9.4308381424504674E-6</v>
+        <f t="shared" ref="E19" si="49">D19/10</f>
+        <v>4.0000000000000007E-6</v>
       </c>
       <c r="F19" s="1">
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="G19" s="1">
-        <v>9.1206383510351521E-6</v>
+        <f t="shared" ref="G19" si="50">F19/10</f>
+        <v>1.5000000000000002E-6</v>
       </c>
       <c r="H19" s="1">
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="I19" s="1">
-        <v>4.8506542485757792E-6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+        <f t="shared" ref="I19" si="51">H19/10</f>
+        <v>1.5000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -3728,28 +3808,32 @@
         <v>7.4226978273101067E-5</v>
       </c>
       <c r="C20" s="1">
-        <v>7.2802740104627959E-6</v>
+        <f t="shared" si="0"/>
+        <v>7.4226978273101063E-6</v>
       </c>
       <c r="D20" s="1">
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="E20" s="1">
-        <v>6.9394426605035223E-6</v>
+        <f t="shared" ref="E20" si="52">D20/10</f>
+        <v>4.0000000000000007E-6</v>
       </c>
       <c r="F20" s="1">
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="G20" s="1">
-        <v>6.7148396165000207E-6</v>
+        <f t="shared" ref="G20" si="53">F20/10</f>
+        <v>1.5000000000000002E-6</v>
       </c>
       <c r="H20" s="1">
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="I20" s="1">
-        <v>3.6379906864318344E-6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+        <f t="shared" ref="I20" si="54">H20/10</f>
+        <v>1.5000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -3757,28 +3841,32 @@
         <v>1.2400555997080529E-5</v>
       </c>
       <c r="C21" s="1">
-        <v>1.2133790017437994E-6</v>
+        <f t="shared" si="0"/>
+        <v>1.2400555997080528E-6</v>
       </c>
       <c r="D21" s="1">
         <v>1.1891705792304714E-5</v>
       </c>
       <c r="E21" s="1">
-        <v>1.158988260905376E-6</v>
+        <f t="shared" ref="E21" si="55">D21/10</f>
+        <v>1.1891705792304714E-6</v>
       </c>
       <c r="F21" s="1">
         <v>1.1317146279096302E-5</v>
       </c>
       <c r="G21" s="1">
-        <v>1.1069754930102333E-6</v>
+        <f t="shared" ref="G21" si="56">F21/10</f>
+        <v>1.1317146279096303E-6</v>
       </c>
       <c r="H21" s="1">
         <v>1.0831391021434082E-5</v>
       </c>
       <c r="I21" s="1">
-        <v>6.063317810719724E-7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+        <f t="shared" ref="I21" si="57">H21/10</f>
+        <v>1.0831391021434082E-6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -3786,28 +3874,32 @@
         <v>4.9602223988322119E-4</v>
       </c>
       <c r="C22" s="1">
-        <v>4.8535160069751977E-5</v>
+        <f t="shared" si="0"/>
+        <v>4.9602223988322116E-5</v>
       </c>
       <c r="D22" s="1">
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="E22" s="1">
-        <v>4.635953043621504E-5</v>
+        <f t="shared" ref="E22" si="58">D22/10</f>
+        <v>4.0000000000000007E-6</v>
       </c>
       <c r="F22" s="1">
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="G22" s="1">
-        <v>4.4279019720409334E-5</v>
+        <f t="shared" ref="G22" si="59">F22/10</f>
+        <v>1.5000000000000002E-6</v>
       </c>
       <c r="H22" s="1">
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="I22" s="1">
-        <v>2.4253271242878896E-5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+        <f t="shared" ref="I22" si="60">H22/10</f>
+        <v>1.5000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -3815,83 +3907,95 @@
         <v>1.3227259730219232E-5</v>
       </c>
       <c r="C23" s="1">
-        <v>1.2942709351933861E-6</v>
+        <f t="shared" si="0"/>
+        <v>1.3227259730219233E-6</v>
       </c>
       <c r="D23" s="1">
         <v>5.3333333333333337E-6</v>
       </c>
       <c r="E23" s="1">
-        <v>1.2362541449657345E-6</v>
+        <f t="shared" ref="E23" si="61">D23/10</f>
+        <v>5.3333333333333334E-7</v>
       </c>
       <c r="F23" s="1">
         <v>2.0000000000000003E-6</v>
       </c>
       <c r="G23" s="1">
-        <v>1.1807738592109156E-6</v>
+        <f t="shared" ref="G23" si="62">F23/10</f>
+        <v>2.0000000000000004E-7</v>
       </c>
       <c r="H23" s="1">
         <v>2.0000000000000003E-6</v>
       </c>
       <c r="I23" s="1">
-        <v>6.4675389981010385E-7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
+        <f t="shared" ref="I23" si="63">H23/10</f>
+        <v>2.0000000000000004E-7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B24" s="1">
         <v>1.2380938429117256E-5</v>
       </c>
       <c r="C24" s="1">
-        <v>1.2170885848263472E-6</v>
+        <f t="shared" si="0"/>
+        <v>1.2380938429117257E-6</v>
       </c>
       <c r="D24" s="1">
         <v>1.1953114268202172E-5</v>
       </c>
       <c r="E24" s="1">
-        <v>1.1771608418890704E-6</v>
+        <f t="shared" ref="E24" si="64">D24/10</f>
+        <v>1.1953114268202171E-6</v>
       </c>
       <c r="F24" s="1">
         <v>1.1671453825073604E-5</v>
       </c>
       <c r="G24" s="1">
-        <v>1.1416206196550427E-6</v>
+        <f t="shared" ref="G24" si="65">F24/10</f>
+        <v>1.1671453825073603E-6</v>
       </c>
       <c r="H24" s="1">
         <v>1.1105118894153889E-5</v>
       </c>
       <c r="I24" s="1">
-        <v>6.063317810719724E-7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
+        <f t="shared" ref="I24" si="66">H24/10</f>
+        <v>1.1105118894153888E-6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="1">
         <v>4.9562944216525952E-4</v>
       </c>
       <c r="C25" s="1">
-        <v>4.8388080342989631E-5</v>
+        <f t="shared" si="0"/>
+        <v>4.9562944216525955E-5</v>
       </c>
       <c r="D25" s="1">
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="E25" s="1">
-        <v>4.6718817598801645E-5</v>
+        <f t="shared" ref="E25" si="67">D25/10</f>
+        <v>4.0000000000000007E-6</v>
       </c>
       <c r="F25" s="1">
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="G25" s="1">
-        <v>4.5480665161870684E-5</v>
+        <f t="shared" ref="G25" si="68">F25/10</f>
+        <v>1.5000000000000002E-6</v>
       </c>
       <c r="H25" s="1">
         <v>1.5000000000000002E-5</v>
       </c>
       <c r="I25" s="1">
-        <v>2.4253271242878896E-5</v>
+        <f t="shared" ref="I25" si="69">H25/10</f>
+        <v>1.5000000000000002E-6</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -3900,35 +4004,38 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
-      <c r="Q25" s="6"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A26" s="4" t="s">
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B26" s="1">
         <v>1.2500000000000002E-5</v>
       </c>
       <c r="C26" s="1">
-        <v>1.2500000000000012E-6</v>
+        <f t="shared" si="0"/>
+        <v>1.2500000000000003E-6</v>
       </c>
       <c r="D26" s="1">
         <v>1.2500000000000002E-5</v>
       </c>
       <c r="E26" s="1">
-        <v>1.2500000000000012E-6</v>
+        <f t="shared" ref="E26" si="70">D26/10</f>
+        <v>1.2500000000000003E-6</v>
       </c>
       <c r="F26" s="1">
         <v>1.2500000000000002E-5</v>
       </c>
       <c r="G26" s="1">
-        <v>1.2500000000000012E-6</v>
+        <f t="shared" ref="G26" si="71">F26/10</f>
+        <v>1.2500000000000003E-6</v>
       </c>
       <c r="H26" s="1">
         <v>1.2500000000000002E-5</v>
       </c>
       <c r="I26" s="1">
-        <v>1.2500000000000012E-6</v>
+        <f t="shared" ref="I26" si="72">H26/10</f>
+        <v>1.2500000000000003E-6</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -3938,149 +4045,169 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B27" s="1">
         <v>1.2500000000000002E-5</v>
       </c>
       <c r="C27" s="1">
-        <v>1.2500000000000012E-6</v>
+        <f t="shared" si="0"/>
+        <v>1.2500000000000003E-6</v>
       </c>
       <c r="D27" s="1">
         <v>1.2500000000000002E-5</v>
       </c>
       <c r="E27" s="1">
-        <v>1.2500000000000012E-6</v>
+        <f t="shared" ref="E27" si="73">D27/10</f>
+        <v>1.2500000000000003E-6</v>
       </c>
       <c r="F27" s="1">
         <v>1.2500000000000002E-5</v>
       </c>
       <c r="G27" s="1">
-        <v>1.2500000000000012E-6</v>
+        <f t="shared" ref="G27" si="74">F27/10</f>
+        <v>1.2500000000000003E-6</v>
       </c>
       <c r="H27" s="1">
         <v>1.2500000000000002E-5</v>
       </c>
       <c r="I27" s="1">
-        <v>1.2500000000000012E-6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A28" s="4" t="s">
+        <f t="shared" ref="I27" si="75">H27/10</f>
+        <v>1.2500000000000003E-6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B28" s="1">
         <v>1.2500000000000002E-5</v>
       </c>
       <c r="C28" s="1">
-        <v>1.2500000000000012E-6</v>
+        <f t="shared" si="0"/>
+        <v>1.2500000000000003E-6</v>
       </c>
       <c r="D28" s="1">
         <v>1.2500000000000002E-5</v>
       </c>
       <c r="E28" s="1">
-        <v>1.2500000000000012E-6</v>
+        <f t="shared" ref="E28" si="76">D28/10</f>
+        <v>1.2500000000000003E-6</v>
       </c>
       <c r="F28" s="1">
         <v>1.2500000000000002E-5</v>
       </c>
       <c r="G28" s="1">
-        <v>1.2500000000000012E-6</v>
+        <f t="shared" ref="G28" si="77">F28/10</f>
+        <v>1.2500000000000003E-6</v>
       </c>
       <c r="H28" s="1">
         <v>1.2500000000000002E-5</v>
       </c>
       <c r="I28" s="1">
-        <v>1.2500000000000012E-6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
+        <f t="shared" ref="I28" si="78">H28/10</f>
+        <v>1.2500000000000003E-6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="1">
         <v>1.2500000000000002E-5</v>
       </c>
       <c r="C29" s="1">
-        <v>1.2489952591188223E-6</v>
+        <f t="shared" si="0"/>
+        <v>1.2500000000000003E-6</v>
       </c>
       <c r="D29" s="1">
         <v>1.192668317934468E-5</v>
       </c>
       <c r="E29" s="1">
-        <v>1.0993135384268758E-6</v>
+        <f t="shared" ref="E29" si="79">D29/10</f>
+        <v>1.1926683179344681E-6</v>
       </c>
       <c r="F29" s="1">
         <v>1.0540661459630418E-5</v>
       </c>
       <c r="G29" s="1">
-        <v>1.0306480610026276E-6</v>
+        <f t="shared" ref="G29" si="80">F29/10</f>
+        <v>1.0540661459630418E-6</v>
       </c>
       <c r="H29" s="1">
         <v>1.0255982148144338E-5</v>
       </c>
       <c r="I29" s="1">
-        <v>6.063317810719724E-7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
+        <f t="shared" ref="I29" si="81">H29/10</f>
+        <v>1.0255982148144339E-6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="1">
         <v>2.4530160436247174E-5</v>
       </c>
       <c r="C30" s="1">
-        <v>2.4048881509400927E-6</v>
+        <f t="shared" si="0"/>
+        <v>2.4530160436247172E-6</v>
       </c>
       <c r="D30" s="1">
         <v>7.9999999999999996E-6</v>
       </c>
       <c r="E30" s="1">
-        <v>2.2649350822873624E-6</v>
+        <f t="shared" ref="E30" si="82">D30/10</f>
+        <v>7.9999999999999996E-7</v>
       </c>
       <c r="F30" s="1">
         <v>3.0000000000000001E-6</v>
       </c>
       <c r="G30" s="1">
-        <v>2.2000069307718571E-6</v>
+        <f t="shared" ref="G30" si="83">F30/10</f>
+        <v>2.9999999999999999E-7</v>
       </c>
       <c r="H30" s="1">
         <v>3.0000000000000001E-6</v>
       </c>
       <c r="I30" s="1">
-        <v>1.2126635621439448E-6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A31" s="4" t="s">
+        <f t="shared" ref="I30" si="84">H30/10</f>
+        <v>2.9999999999999999E-7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="1">
         <v>2.4761876858234513E-5</v>
       </c>
       <c r="C31" s="1">
-        <v>2.4157511964427715E-6</v>
+        <f t="shared" si="0"/>
+        <v>2.4761876858234514E-6</v>
       </c>
       <c r="D31" s="1">
         <v>7.9999999999999996E-6</v>
       </c>
       <c r="E31" s="1">
-        <v>2.3212124391588087E-6</v>
+        <f t="shared" ref="E31" si="85">D31/10</f>
+        <v>7.9999999999999996E-7</v>
       </c>
       <c r="F31" s="1">
         <v>3.0000000000000001E-6</v>
       </c>
       <c r="G31" s="1">
-        <v>2.2740332580935344E-6</v>
+        <f t="shared" ref="G31" si="86">F31/10</f>
+        <v>2.9999999999999999E-7</v>
       </c>
       <c r="H31" s="1">
         <v>3.0000000000000001E-6</v>
       </c>
       <c r="I31" s="1">
-        <v>1.2126635621439448E-6</v>
+        <f t="shared" ref="I31" si="87">H31/10</f>
+        <v>2.9999999999999999E-7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New figures for second review. Added saving subsidence results. Added updates to code. Calibration and Validation of Pastas.
</commit_message>
<xml_diff>
--- a/inputs/SUBParameters.xlsx
+++ b/inputs/SUBParameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtsoonthornran\BKKSubPastasModels\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DDDED4-ABBC-40CF-9E6D-E4386650142A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DBAF95-CB7E-4F92-89F0-27C12B1BCAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-50" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="K" sheetId="21" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="32">
   <si>
     <t>VSC</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>LCBKK003</t>
-  </si>
-  <si>
-    <t>LCBKK004</t>
   </si>
   <si>
     <t>LCBKK005</t>
@@ -107,25 +104,16 @@
     <t>LCBKK021</t>
   </si>
   <si>
-    <t>LCBKK022</t>
-  </si>
-  <si>
     <t>LCBKK026</t>
   </si>
   <si>
     <t>LCBKK036</t>
   </si>
   <si>
-    <t>LCBKK037</t>
-  </si>
-  <si>
     <t>LCBKK038</t>
   </si>
   <si>
     <t>LCBKK041</t>
-  </si>
-  <si>
-    <t>LCSPK005</t>
   </si>
   <si>
     <t>LCSPK007</t>
@@ -147,15 +135,6 @@
   </si>
   <si>
     <t>LCNBI007</t>
-  </si>
-  <si>
-    <t>LCNPT003</t>
-  </si>
-  <si>
-    <t>LCNPT005</t>
-  </si>
-  <si>
-    <t>LCSKN004</t>
   </si>
 </sst>
 </file>
@@ -488,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -562,25 +541,25 @@
         <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>5.0040000000000002E-5</v>
+        <v>1.0008E-4</v>
       </c>
       <c r="C3" s="1">
         <v>13</v>
       </c>
       <c r="D3" s="1">
-        <v>2.5100000000000001E-6</v>
+        <v>5.0200000000000002E-6</v>
       </c>
       <c r="E3" s="1">
         <v>70</v>
       </c>
       <c r="F3" s="1">
-        <v>2.1E-7</v>
+        <v>4.2E-7</v>
       </c>
       <c r="G3" s="1">
         <v>62</v>
       </c>
       <c r="H3" s="1">
-        <v>5.0250000000000006E-7</v>
+        <v>1.0050000000000001E-6</v>
       </c>
       <c r="I3" s="1">
         <v>67</v>
@@ -591,25 +570,25 @@
         <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>1.0008E-4</v>
+        <v>7.5060000000000003E-5</v>
       </c>
       <c r="C4" s="1">
         <v>13</v>
       </c>
       <c r="D4" s="1">
-        <v>5.0200000000000002E-6</v>
+        <v>3.765E-6</v>
       </c>
       <c r="E4" s="1">
         <v>70</v>
       </c>
       <c r="F4" s="1">
-        <v>4.2E-7</v>
+        <v>3.1499999999999995E-7</v>
       </c>
       <c r="G4" s="1">
         <v>62</v>
       </c>
       <c r="H4" s="1">
-        <v>1.0050000000000001E-6</v>
+        <v>7.5374999999999998E-7</v>
       </c>
       <c r="I4" s="1">
         <v>67</v>
@@ -620,25 +599,25 @@
         <v>12</v>
       </c>
       <c r="B5" s="1">
-        <v>7.5060000000000003E-5</v>
+        <v>2.502E-7</v>
       </c>
       <c r="C5" s="1">
         <v>13</v>
       </c>
       <c r="D5" s="1">
-        <v>3.765E-6</v>
+        <v>1.2550000000000001E-7</v>
       </c>
       <c r="E5" s="1">
         <v>70</v>
       </c>
       <c r="F5" s="1">
-        <v>3.1499999999999995E-7</v>
+        <v>1.05E-7</v>
       </c>
       <c r="G5" s="1">
         <v>62</v>
       </c>
       <c r="H5" s="1">
-        <v>7.5374999999999998E-7</v>
+        <v>2.5124999999999998E-8</v>
       </c>
       <c r="I5" s="1">
         <v>67</v>
@@ -649,25 +628,25 @@
         <v>13</v>
       </c>
       <c r="B6" s="1">
-        <v>2.502E-7</v>
+        <v>7.5060000000000003E-5</v>
       </c>
       <c r="C6" s="1">
         <v>13</v>
       </c>
       <c r="D6" s="1">
-        <v>1.2550000000000001E-7</v>
+        <v>3.765E-6</v>
       </c>
       <c r="E6" s="1">
         <v>70</v>
       </c>
       <c r="F6" s="1">
-        <v>1.05E-7</v>
+        <v>3.1499999999999995E-7</v>
       </c>
       <c r="G6" s="1">
         <v>62</v>
       </c>
       <c r="H6" s="1">
-        <v>2.5124999999999998E-8</v>
+        <v>7.5374999999999998E-7</v>
       </c>
       <c r="I6" s="1">
         <v>67</v>
@@ -678,25 +657,25 @@
         <v>14</v>
       </c>
       <c r="B7" s="1">
-        <v>7.5060000000000003E-5</v>
+        <v>2.5020000000000004E-6</v>
       </c>
       <c r="C7" s="1">
         <v>13</v>
       </c>
       <c r="D7" s="1">
-        <v>3.765E-6</v>
+        <v>1.2550000000000001E-6</v>
       </c>
       <c r="E7" s="1">
         <v>70</v>
       </c>
       <c r="F7" s="1">
-        <v>3.1499999999999995E-7</v>
+        <v>1.05E-7</v>
       </c>
       <c r="G7" s="1">
         <v>62</v>
       </c>
       <c r="H7" s="1">
-        <v>7.5374999999999998E-7</v>
+        <v>2.5125000000000003E-7</v>
       </c>
       <c r="I7" s="1">
         <v>67</v>
@@ -707,25 +686,25 @@
         <v>15</v>
       </c>
       <c r="B8" s="1">
-        <v>2.5020000000000004E-6</v>
+        <v>4.5036E-5</v>
       </c>
       <c r="C8" s="1">
         <v>13</v>
       </c>
       <c r="D8" s="1">
-        <v>1.2550000000000001E-6</v>
+        <v>2.2589999999999999E-6</v>
       </c>
       <c r="E8" s="1">
         <v>70</v>
       </c>
       <c r="F8" s="1">
-        <v>1.05E-7</v>
+        <v>1.8899999999999999E-7</v>
       </c>
       <c r="G8" s="1">
         <v>62</v>
       </c>
       <c r="H8" s="1">
-        <v>2.5125000000000003E-7</v>
+        <v>4.5224999999999999E-7</v>
       </c>
       <c r="I8" s="1">
         <v>67</v>
@@ -736,7 +715,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="1">
-        <v>4.5036E-5</v>
+        <v>4.5036000000000004E-6</v>
       </c>
       <c r="C9" s="1">
         <v>13</v>
@@ -820,28 +799,28 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1">
-        <v>4.5036000000000004E-6</v>
+        <v>3.5028000000000006E-6</v>
       </c>
       <c r="C12" s="1">
         <v>13</v>
       </c>
       <c r="D12" s="1">
-        <v>2.2589999999999999E-6</v>
+        <v>1.7570000000000003E-6</v>
       </c>
       <c r="E12" s="1">
         <v>70</v>
       </c>
       <c r="F12" s="1">
-        <v>1.8899999999999999E-7</v>
+        <v>1.4700000000000001E-7</v>
       </c>
       <c r="G12" s="1">
         <v>62</v>
       </c>
       <c r="H12" s="1">
-        <v>4.5224999999999999E-7</v>
+        <v>3.5175000000000006E-7</v>
       </c>
       <c r="I12" s="1">
         <v>67</v>
@@ -849,28 +828,28 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1">
-        <v>3.5028000000000006E-6</v>
+        <v>4.5036E-5</v>
       </c>
       <c r="C13" s="1">
         <v>13</v>
       </c>
       <c r="D13" s="1">
-        <v>1.7570000000000003E-6</v>
+        <v>2.2589999999999999E-6</v>
       </c>
       <c r="E13" s="1">
         <v>70</v>
       </c>
       <c r="F13" s="1">
-        <v>1.4700000000000001E-7</v>
+        <v>1.8899999999999999E-7</v>
       </c>
       <c r="G13" s="1">
         <v>62</v>
       </c>
       <c r="H13" s="1">
-        <v>3.5175000000000006E-7</v>
+        <v>4.5224999999999999E-7</v>
       </c>
       <c r="I13" s="1">
         <v>67</v>
@@ -878,28 +857,28 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1">
-        <v>4.5036E-5</v>
+        <v>5.0040000000000007E-6</v>
       </c>
       <c r="C14" s="1">
         <v>13</v>
       </c>
       <c r="D14" s="1">
-        <v>2.2589999999999999E-6</v>
+        <v>2.5100000000000001E-6</v>
       </c>
       <c r="E14" s="1">
         <v>70</v>
       </c>
       <c r="F14" s="1">
-        <v>1.8899999999999999E-7</v>
+        <v>2.1E-7</v>
       </c>
       <c r="G14" s="1">
         <v>62</v>
       </c>
       <c r="H14" s="1">
-        <v>4.5224999999999999E-7</v>
+        <v>5.0250000000000006E-7</v>
       </c>
       <c r="I14" s="1">
         <v>67</v>
@@ -939,25 +918,25 @@
         <v>21</v>
       </c>
       <c r="B16" s="1">
-        <v>5.0040000000000007E-6</v>
+        <v>2.5020000000000001E-5</v>
       </c>
       <c r="C16" s="1">
         <v>13</v>
       </c>
       <c r="D16" s="1">
-        <v>2.5100000000000001E-6</v>
+        <v>1.2550000000000001E-6</v>
       </c>
       <c r="E16" s="1">
         <v>70</v>
       </c>
       <c r="F16" s="1">
-        <v>2.1E-7</v>
+        <v>1.05E-7</v>
       </c>
       <c r="G16" s="1">
         <v>62</v>
       </c>
       <c r="H16" s="1">
-        <v>5.0250000000000006E-7</v>
+        <v>2.5125000000000003E-7</v>
       </c>
       <c r="I16" s="1">
         <v>67</v>
@@ -965,28 +944,28 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1">
-        <v>2.5020000000000001E-5</v>
+        <v>4.5036E-5</v>
       </c>
       <c r="C17" s="1">
         <v>13</v>
       </c>
       <c r="D17" s="1">
-        <v>1.2550000000000001E-6</v>
+        <v>2.2589999999999999E-6</v>
       </c>
       <c r="E17" s="1">
         <v>70</v>
       </c>
       <c r="F17" s="1">
-        <v>1.05E-7</v>
+        <v>1.8899999999999999E-7</v>
       </c>
       <c r="G17" s="1">
         <v>62</v>
       </c>
       <c r="H17" s="1">
-        <v>2.5125000000000003E-7</v>
+        <v>4.5224999999999999E-7</v>
       </c>
       <c r="I17" s="1">
         <v>67</v>
@@ -994,28 +973,28 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1">
-        <v>2.5020000000000001E-5</v>
+        <v>7.5060000000000003E-5</v>
       </c>
       <c r="C18" s="1">
         <v>13</v>
       </c>
       <c r="D18" s="1">
-        <v>1.2550000000000001E-6</v>
+        <v>3.765E-6</v>
       </c>
       <c r="E18" s="1">
         <v>70</v>
       </c>
       <c r="F18" s="1">
-        <v>1.05E-7</v>
+        <v>3.1499999999999995E-7</v>
       </c>
       <c r="G18" s="1">
         <v>62</v>
       </c>
       <c r="H18" s="1">
-        <v>2.5125000000000003E-7</v>
+        <v>7.5374999999999998E-7</v>
       </c>
       <c r="I18" s="1">
         <v>67</v>
@@ -1023,10 +1002,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1">
-        <v>4.5036E-5</v>
+        <v>4.5036000000000004E-6</v>
       </c>
       <c r="C19" s="1">
         <v>13</v>
@@ -1055,33 +1034,33 @@
         <v>24</v>
       </c>
       <c r="B20" s="1">
-        <v>7.5060000000000003E-5</v>
+        <v>4.5036000000000004E-6</v>
       </c>
       <c r="C20" s="1">
         <v>13</v>
       </c>
       <c r="D20" s="1">
-        <v>3.765E-6</v>
+        <v>2.2589999999999999E-6</v>
       </c>
       <c r="E20" s="1">
         <v>70</v>
       </c>
       <c r="F20" s="1">
-        <v>3.1499999999999995E-7</v>
+        <v>1.8899999999999999E-7</v>
       </c>
       <c r="G20" s="1">
         <v>62</v>
       </c>
       <c r="H20" s="1">
-        <v>7.5374999999999998E-7</v>
+        <v>4.5224999999999999E-7</v>
       </c>
       <c r="I20" s="1">
         <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>25</v>
+      <c r="A21" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B21" s="1">
         <v>4.5036E-5</v>
@@ -1109,40 +1088,40 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>26</v>
+      <c r="A22" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B22" s="1">
-        <v>4.5036000000000004E-6</v>
+        <v>2.502E-7</v>
       </c>
       <c r="C22" s="1">
         <v>13</v>
       </c>
       <c r="D22" s="1">
-        <v>2.2589999999999999E-6</v>
+        <v>1.2550000000000001E-7</v>
       </c>
       <c r="E22" s="1">
         <v>70</v>
       </c>
       <c r="F22" s="1">
-        <v>1.8899999999999999E-7</v>
+        <v>1.05E-7</v>
       </c>
       <c r="G22" s="1">
         <v>62</v>
       </c>
       <c r="H22" s="1">
-        <v>4.5224999999999999E-7</v>
+        <v>2.5125000000000003E-7</v>
       </c>
       <c r="I22" s="1">
         <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>27</v>
+      <c r="A23" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B23" s="1">
-        <v>4.5036000000000004E-6</v>
+        <v>4.5036E-5</v>
       </c>
       <c r="C23" s="1">
         <v>13</v>
@@ -1168,10 +1147,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1">
-        <v>4.5036E-5</v>
+        <v>4.5036000000000004E-6</v>
       </c>
       <c r="C24" s="1">
         <v>13</v>
@@ -1192,209 +1171,6 @@
         <v>4.5224999999999999E-7</v>
       </c>
       <c r="I24" s="1">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="1">
-        <v>2.502E-7</v>
-      </c>
-      <c r="C25" s="1">
-        <v>13</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1.2550000000000001E-7</v>
-      </c>
-      <c r="E25" s="1">
-        <v>70</v>
-      </c>
-      <c r="F25" s="1">
-        <v>1.05E-7</v>
-      </c>
-      <c r="G25" s="1">
-        <v>62</v>
-      </c>
-      <c r="H25" s="1">
-        <v>2.5125000000000003E-7</v>
-      </c>
-      <c r="I25" s="1">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="1">
-        <v>4.5036E-5</v>
-      </c>
-      <c r="C26" s="1">
-        <v>13</v>
-      </c>
-      <c r="D26" s="1">
-        <v>2.2589999999999999E-6</v>
-      </c>
-      <c r="E26" s="1">
-        <v>70</v>
-      </c>
-      <c r="F26" s="1">
-        <v>1.8899999999999999E-7</v>
-      </c>
-      <c r="G26" s="1">
-        <v>62</v>
-      </c>
-      <c r="H26" s="1">
-        <v>4.5224999999999999E-7</v>
-      </c>
-      <c r="I26" s="1">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="1">
-        <v>4.5036E-5</v>
-      </c>
-      <c r="C27" s="1">
-        <v>13</v>
-      </c>
-      <c r="D27" s="1">
-        <v>2.2589999999999999E-6</v>
-      </c>
-      <c r="E27" s="1">
-        <v>70</v>
-      </c>
-      <c r="F27" s="1">
-        <v>1.8899999999999999E-7</v>
-      </c>
-      <c r="G27" s="1">
-        <v>62</v>
-      </c>
-      <c r="H27" s="1">
-        <v>4.5224999999999999E-7</v>
-      </c>
-      <c r="I27" s="1">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="1">
-        <v>4.5036E-5</v>
-      </c>
-      <c r="C28" s="1">
-        <v>13</v>
-      </c>
-      <c r="D28" s="1">
-        <v>2.2589999999999999E-6</v>
-      </c>
-      <c r="E28" s="1">
-        <v>70</v>
-      </c>
-      <c r="F28" s="1">
-        <v>1.8899999999999999E-7</v>
-      </c>
-      <c r="G28" s="1">
-        <v>62</v>
-      </c>
-      <c r="H28" s="1">
-        <v>4.5224999999999999E-7</v>
-      </c>
-      <c r="I28" s="1">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1">
-        <v>4.5036E-5</v>
-      </c>
-      <c r="C29" s="1">
-        <v>13</v>
-      </c>
-      <c r="D29" s="1">
-        <v>2.2589999999999999E-6</v>
-      </c>
-      <c r="E29" s="1">
-        <v>70</v>
-      </c>
-      <c r="F29" s="1">
-        <v>1.8899999999999999E-7</v>
-      </c>
-      <c r="G29" s="1">
-        <v>62</v>
-      </c>
-      <c r="H29" s="1">
-        <v>4.5224999999999999E-7</v>
-      </c>
-      <c r="I29" s="1">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1">
-        <v>4.5036E-5</v>
-      </c>
-      <c r="C30" s="1">
-        <v>13</v>
-      </c>
-      <c r="D30" s="1">
-        <v>2.2589999999999999E-6</v>
-      </c>
-      <c r="E30" s="1">
-        <v>70</v>
-      </c>
-      <c r="F30" s="1">
-        <v>1.8899999999999999E-7</v>
-      </c>
-      <c r="G30" s="1">
-        <v>62</v>
-      </c>
-      <c r="H30" s="1">
-        <v>4.5224999999999999E-7</v>
-      </c>
-      <c r="I30" s="1">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1">
-        <v>4.5036000000000004E-6</v>
-      </c>
-      <c r="C31" s="1">
-        <v>13</v>
-      </c>
-      <c r="D31" s="1">
-        <v>2.2589999999999999E-6</v>
-      </c>
-      <c r="E31" s="1">
-        <v>70</v>
-      </c>
-      <c r="F31" s="1">
-        <v>1.8899999999999999E-7</v>
-      </c>
-      <c r="G31" s="1">
-        <v>62</v>
-      </c>
-      <c r="H31" s="1">
-        <v>4.5224999999999999E-7</v>
-      </c>
-      <c r="I31" s="1">
         <v>67</v>
       </c>
     </row>
@@ -1406,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1478,28 +1254,28 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C3">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D3">
-        <v>25.5</v>
+        <v>19.5</v>
       </c>
       <c r="E3">
-        <v>42</v>
+        <v>52.5</v>
       </c>
       <c r="F3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3">
-        <v>28.5</v>
+        <v>51</v>
       </c>
       <c r="H3">
-        <v>6.1</v>
+        <v>19</v>
       </c>
       <c r="I3">
-        <v>6.7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -1507,28 +1283,28 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C4">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D4">
-        <v>19.5</v>
+        <v>30</v>
       </c>
       <c r="E4">
-        <v>52.5</v>
+        <v>42</v>
       </c>
       <c r="F4">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G4">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="H4">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="I4">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -1536,28 +1312,28 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>33</v>
+        <v>25.8</v>
       </c>
       <c r="C5">
-        <v>21</v>
+        <v>41.2</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <v>16.5</v>
       </c>
       <c r="E5">
-        <v>42</v>
+        <v>50.3</v>
       </c>
       <c r="F5">
-        <v>13</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="G5">
-        <v>59</v>
+        <v>56.1</v>
       </c>
       <c r="H5">
-        <v>5</v>
+        <v>6.1</v>
       </c>
       <c r="I5">
-        <v>18</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -1565,28 +1341,28 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>25.8</v>
+        <v>38.1</v>
       </c>
       <c r="C6">
-        <v>41.2</v>
+        <v>15.2</v>
       </c>
       <c r="D6">
-        <v>16.5</v>
+        <v>6.7</v>
       </c>
       <c r="E6">
-        <v>50.3</v>
+        <v>65.2</v>
       </c>
       <c r="F6">
-        <v>17.399999999999999</v>
+        <v>12.5</v>
       </c>
       <c r="G6">
-        <v>56.1</v>
+        <v>19.8</v>
       </c>
       <c r="H6">
-        <v>6.1</v>
+        <v>4.3</v>
       </c>
       <c r="I6">
-        <v>6.7</v>
+        <v>35.9</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -1594,28 +1370,28 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <v>38.1</v>
+        <v>27</v>
       </c>
       <c r="C7">
-        <v>15.2</v>
+        <v>58</v>
       </c>
       <c r="D7">
-        <v>6.7</v>
+        <v>23.6</v>
       </c>
       <c r="E7">
-        <v>65.2</v>
+        <v>47.2</v>
       </c>
       <c r="F7">
-        <v>12.5</v>
+        <v>13.5</v>
       </c>
       <c r="G7">
-        <v>19.8</v>
+        <v>27</v>
       </c>
       <c r="H7">
-        <v>4.3</v>
+        <v>3.7</v>
       </c>
       <c r="I7">
-        <v>35.9</v>
+        <v>34.200000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -1623,28 +1399,28 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>27</v>
+        <v>25.1</v>
       </c>
       <c r="C8">
-        <v>58</v>
+        <v>19.8</v>
       </c>
       <c r="D8">
-        <v>23.6</v>
+        <v>45.2</v>
       </c>
       <c r="E8">
-        <v>47.2</v>
+        <v>22.5</v>
       </c>
       <c r="F8">
-        <v>13.5</v>
+        <v>60</v>
       </c>
       <c r="G8">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="H8">
-        <v>3.7</v>
+        <v>20</v>
       </c>
       <c r="I8">
-        <v>34.200000000000003</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -1652,28 +1428,28 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>38.5</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>40.1</v>
       </c>
       <c r="D9">
-        <v>120</v>
+        <v>20.9</v>
       </c>
       <c r="E9">
-        <v>120</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="F9">
-        <v>20</v>
+        <v>10.4</v>
       </c>
       <c r="G9">
-        <v>60</v>
+        <v>55.7</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>8.9</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>19.100000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
@@ -1681,28 +1457,28 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <v>38.5</v>
+        <v>36</v>
       </c>
       <c r="C10">
-        <v>40.1</v>
+        <v>15</v>
       </c>
       <c r="D10">
-        <v>20.9</v>
+        <v>40</v>
       </c>
       <c r="E10">
-        <v>17.399999999999999</v>
+        <v>35</v>
       </c>
       <c r="F10">
-        <v>10.4</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>55.7</v>
+        <v>65</v>
       </c>
       <c r="H10">
-        <v>8.9</v>
+        <v>30</v>
       </c>
       <c r="I10">
-        <v>19.100000000000001</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -1710,115 +1486,115 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <v>36</v>
+        <v>25.8</v>
       </c>
       <c r="C11">
-        <v>15</v>
+        <v>41.2</v>
       </c>
       <c r="D11">
-        <v>40</v>
+        <v>16.5</v>
       </c>
       <c r="E11">
-        <v>35</v>
+        <v>50.3</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="G11">
-        <v>65</v>
+        <v>56.1</v>
       </c>
       <c r="H11">
-        <v>30</v>
+        <v>6.1</v>
       </c>
       <c r="I11">
-        <v>6</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B12">
-        <v>25.8</v>
+        <v>27.7</v>
       </c>
       <c r="C12">
-        <v>41.2</v>
+        <v>19.3</v>
       </c>
       <c r="D12">
-        <v>16.5</v>
+        <v>36</v>
       </c>
       <c r="E12">
-        <v>50.3</v>
+        <v>14.2</v>
       </c>
       <c r="F12">
-        <v>17.399999999999999</v>
+        <v>9.4</v>
       </c>
       <c r="G12">
-        <v>56.1</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="H12">
-        <v>6.1</v>
+        <v>19.2</v>
       </c>
       <c r="I12">
-        <v>6.7</v>
+        <v>72.5</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B13">
-        <v>27.7</v>
+        <v>27</v>
       </c>
       <c r="C13">
-        <v>19.3</v>
+        <v>27</v>
       </c>
       <c r="D13">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="E13">
-        <v>14.2</v>
+        <v>48</v>
       </c>
       <c r="F13">
-        <v>9.4</v>
+        <v>26.2</v>
       </c>
       <c r="G13">
-        <v>36.299999999999997</v>
+        <v>20.8</v>
       </c>
       <c r="H13">
-        <v>19.2</v>
+        <v>11.3</v>
       </c>
       <c r="I13">
-        <v>72.5</v>
+        <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B14">
-        <v>27</v>
+        <v>24.5</v>
       </c>
       <c r="C14">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D14">
-        <v>12</v>
+        <v>39.5</v>
       </c>
       <c r="E14">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="F14">
-        <v>26.2</v>
+        <v>18.5</v>
       </c>
       <c r="G14">
-        <v>20.8</v>
+        <v>41.5</v>
       </c>
       <c r="H14">
-        <v>11.3</v>
+        <v>8</v>
       </c>
       <c r="I14">
-        <v>9.6999999999999993</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
@@ -1826,28 +1602,28 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>24.5</v>
+        <v>18</v>
       </c>
       <c r="C15">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D15">
-        <v>39.5</v>
+        <v>45</v>
       </c>
       <c r="E15">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="F15">
-        <v>18.5</v>
+        <v>39</v>
       </c>
       <c r="G15">
-        <v>41.5</v>
+        <v>54</v>
       </c>
       <c r="H15">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I15">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
@@ -1855,115 +1631,115 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>18</v>
+        <v>25.5</v>
       </c>
       <c r="C16">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D16">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="E16">
-        <v>33</v>
+        <v>34.5</v>
       </c>
       <c r="F16">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="G16">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="H16">
         <v>3</v>
       </c>
       <c r="I16">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B17">
-        <v>29.2</v>
+        <v>42</v>
       </c>
       <c r="C17">
-        <v>18.3</v>
+        <v>6</v>
       </c>
       <c r="D17">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E17">
-        <v>37.799999999999997</v>
+        <v>13.5</v>
       </c>
       <c r="F17">
-        <v>26.2</v>
+        <v>24</v>
       </c>
       <c r="G17">
-        <v>20.8</v>
+        <v>34.5</v>
       </c>
       <c r="H17">
-        <v>11.3</v>
+        <v>51</v>
       </c>
       <c r="I17">
-        <v>9.6999999999999993</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18">
-        <v>25.5</v>
+        <v>28</v>
       </c>
       <c r="C18">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D18">
-        <v>10</v>
+        <v>47.2</v>
       </c>
       <c r="E18">
-        <v>34.5</v>
+        <v>15.8</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="H18">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="I18">
-        <v>130</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B19">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D19">
-        <v>23</v>
+        <v>19.5</v>
       </c>
       <c r="E19">
-        <v>13.5</v>
+        <v>52.5</v>
       </c>
       <c r="F19">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G19">
-        <v>34.5</v>
+        <v>51</v>
       </c>
       <c r="H19">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="I19">
-        <v>18.5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -1971,259 +1747,143 @@
         <v>24</v>
       </c>
       <c r="B20">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>34</v>
+      </c>
+      <c r="D20">
+        <v>19.5</v>
+      </c>
+      <c r="E20">
+        <v>52.5</v>
+      </c>
+      <c r="F20">
+        <v>17</v>
+      </c>
+      <c r="G20">
+        <v>51</v>
+      </c>
+      <c r="H20">
+        <v>19</v>
+      </c>
+      <c r="I20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <v>25</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
         <v>28</v>
       </c>
-      <c r="C20">
-        <v>21</v>
-      </c>
-      <c r="D20">
-        <v>47.2</v>
-      </c>
-      <c r="E20">
-        <v>15.8</v>
-      </c>
-      <c r="F20">
-        <v>28</v>
-      </c>
-      <c r="G20">
-        <v>28</v>
-      </c>
-      <c r="H20">
-        <v>37</v>
-      </c>
-      <c r="I20">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="E21">
+        <v>14</v>
+      </c>
+      <c r="F21">
+        <v>9</v>
+      </c>
+      <c r="G21">
+        <v>55</v>
+      </c>
+      <c r="H21">
+        <v>30</v>
+      </c>
+      <c r="I21">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22">
+        <v>23.2</v>
+      </c>
+      <c r="C22">
+        <v>39</v>
+      </c>
+      <c r="D22">
+        <v>7.9</v>
+      </c>
+      <c r="E22">
+        <v>40.9</v>
+      </c>
+      <c r="F22">
+        <v>7.5</v>
+      </c>
+      <c r="G22">
+        <v>22.3</v>
+      </c>
+      <c r="H22">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="I22">
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B21">
-        <v>22</v>
-      </c>
-      <c r="C21">
-        <v>34</v>
-      </c>
-      <c r="D21">
-        <v>19.5</v>
-      </c>
-      <c r="E21">
-        <v>52.5</v>
-      </c>
-      <c r="F21">
-        <v>17</v>
-      </c>
-      <c r="G21">
-        <v>51</v>
-      </c>
-      <c r="H21">
-        <v>19</v>
-      </c>
-      <c r="I21">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22">
-        <v>22</v>
-      </c>
-      <c r="C22">
-        <v>34</v>
-      </c>
-      <c r="D22">
-        <v>19.5</v>
-      </c>
-      <c r="E22">
-        <v>52.5</v>
-      </c>
-      <c r="F22">
-        <v>17</v>
-      </c>
-      <c r="G22">
-        <v>51</v>
-      </c>
-      <c r="H22">
-        <v>19</v>
-      </c>
-      <c r="I22">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>27</v>
-      </c>
       <c r="B23">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C23">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D23">
-        <v>19.5</v>
+        <v>70</v>
       </c>
       <c r="E23">
-        <v>52.5</v>
+        <v>30</v>
       </c>
       <c r="F23">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G23">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="H23">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I23">
-        <v>11</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B24">
-        <v>25</v>
+        <v>25.5</v>
       </c>
       <c r="C24">
-        <v>20</v>
+        <v>37.5</v>
       </c>
       <c r="D24">
-        <v>28</v>
+        <v>33.5</v>
       </c>
       <c r="E24">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F24">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G24">
-        <v>55</v>
+        <v>21.5</v>
       </c>
       <c r="H24">
-        <v>30</v>
+        <v>11.5</v>
       </c>
       <c r="I24">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25">
-        <v>23.2</v>
-      </c>
-      <c r="C25">
-        <v>39</v>
-      </c>
-      <c r="D25">
-        <v>7.9</v>
-      </c>
-      <c r="E25">
-        <v>40.9</v>
-      </c>
-      <c r="F25">
-        <v>7.5</v>
-      </c>
-      <c r="G25">
-        <v>22.3</v>
-      </c>
-      <c r="H25">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="I25">
-        <v>76.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>120</v>
-      </c>
-      <c r="E26">
-        <v>120</v>
-      </c>
-      <c r="F26">
-        <v>20</v>
-      </c>
-      <c r="G26">
-        <v>60</v>
-      </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
-      <c r="I26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27">
-        <v>50</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>70</v>
-      </c>
-      <c r="E27">
-        <v>30</v>
-      </c>
-      <c r="F27">
-        <v>20</v>
-      </c>
-      <c r="G27">
-        <v>20</v>
-      </c>
-      <c r="H27">
-        <v>20</v>
-      </c>
-      <c r="I27">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28">
-        <v>25.5</v>
-      </c>
-      <c r="C28">
-        <v>37.5</v>
-      </c>
-      <c r="D28">
-        <v>33.5</v>
-      </c>
-      <c r="E28">
-        <v>7</v>
-      </c>
-      <c r="F28">
-        <v>15</v>
-      </c>
-      <c r="G28">
-        <v>21.5</v>
-      </c>
-      <c r="H28">
-        <v>11.5</v>
-      </c>
-      <c r="I28">
         <v>55.5</v>
       </c>
     </row>
@@ -2234,10 +1894,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2316,28 +1976,28 @@
         <v>10</v>
       </c>
       <c r="B3" s="5">
-        <v>4.9484652182067376E-4</v>
+        <v>2.4801111994161061E-3</v>
       </c>
       <c r="C3" s="5">
-        <v>4.8572133008237997E-5</v>
-      </c>
-      <c r="D3" s="5">
-        <v>4.7741898312494817E-4</v>
+        <v>2.426758003487599E-4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="E3" s="5">
-        <v>4.6587219190804714E-5</v>
-      </c>
-      <c r="F3" s="5">
-        <v>4.5633977302917989E-4</v>
+        <v>2.3179765218107521E-4</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3.0000000000000003E-4</v>
       </c>
       <c r="G3" s="5">
-        <v>4.4941205889230356E-5</v>
-      </c>
-      <c r="H3" s="5">
-        <v>4.4420475576615557E-4</v>
+        <v>2.2139509860204666E-4</v>
+      </c>
+      <c r="H3" s="1">
+        <v>3.0000000000000003E-4</v>
       </c>
       <c r="I3" s="5">
-        <v>2.4253271242878896E-5</v>
+        <v>1.2126635621439448E-4</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -2345,22 +2005,22 @@
         <v>11</v>
       </c>
       <c r="B4" s="5">
-        <v>2.4801111994161061E-3</v>
+        <v>2.4683939166376461E-3</v>
       </c>
       <c r="C4" s="5">
-        <v>2.426758003487599E-4</v>
+        <v>2.4175756035617484E-4</v>
       </c>
       <c r="D4" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="E4" s="5">
-        <v>2.3179765218107521E-4</v>
+        <v>2.3131475535011746E-4</v>
       </c>
       <c r="F4" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="G4" s="5">
-        <v>2.2139509860204666E-4</v>
+        <v>2.2167719477749056E-4</v>
       </c>
       <c r="H4" s="1">
         <v>3.0000000000000003E-4</v>
@@ -2374,28 +2034,28 @@
         <v>12</v>
       </c>
       <c r="B5" s="5">
-        <v>2.4683939166376461E-3</v>
+        <v>7.428563057470354E-3</v>
       </c>
       <c r="C5" s="5">
-        <v>2.4175756035617484E-4</v>
+        <v>7.2363430458604477E-4</v>
       </c>
       <c r="D5" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="E5" s="5">
-        <v>2.3131475535011746E-4</v>
+        <v>6.9202649739300676E-4</v>
       </c>
       <c r="F5" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="G5" s="5">
-        <v>2.2167719477749056E-4</v>
+        <v>6.6041682225121106E-4</v>
       </c>
       <c r="H5" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="I5" s="5">
-        <v>1.2126635621439448E-4</v>
+        <v>3.6379906864318341E-4</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -2403,28 +2063,28 @@
         <v>13</v>
       </c>
       <c r="B6" s="5">
-        <v>7.428563057470354E-3</v>
+        <v>1.2312973571959758E-3</v>
       </c>
       <c r="C6" s="5">
-        <v>7.2363430458604477E-4</v>
+        <v>1.2069653912651356E-4</v>
       </c>
       <c r="D6" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="E6" s="5">
-        <v>6.9202649739300676E-4</v>
+        <v>1.1663220402473934E-4</v>
       </c>
       <c r="F6" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="G6" s="5">
-        <v>6.6041682225121106E-4</v>
+        <v>1.1235301472307589E-4</v>
       </c>
       <c r="H6" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="I6" s="5">
-        <v>3.6379906864318341E-4</v>
+        <v>6.0633178107197238E-5</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -2432,28 +2092,28 @@
         <v>14</v>
       </c>
       <c r="B7" s="5">
-        <v>1.2312973571959758E-3</v>
+        <v>3.9587721745653901E-3</v>
       </c>
       <c r="C7" s="5">
-        <v>1.2069653912651356E-4</v>
+        <v>3.8335094292073939E-4</v>
       </c>
       <c r="D7" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="E7" s="5">
-        <v>1.1663220402473934E-4</v>
+        <v>3.6311529104932668E-4</v>
       </c>
       <c r="F7" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="G7" s="5">
-        <v>1.1235301472307589E-4</v>
+        <v>3.515599741109437E-4</v>
       </c>
       <c r="H7" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="I7" s="5">
-        <v>6.0633178107197238E-5</v>
+        <v>1.9402616994303117E-4</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -2461,25 +2121,25 @@
         <v>15</v>
       </c>
       <c r="B8" s="5">
-        <v>3.9587721745653901E-3</v>
+        <v>4.000000000000001E-3</v>
       </c>
       <c r="C8" s="5">
-        <v>3.8335094292073939E-4</v>
+        <v>3.9967848291802316E-4</v>
       </c>
       <c r="D8" s="1">
-        <v>8.0000000000000004E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="E8" s="5">
-        <v>3.6311529104932668E-4</v>
+        <v>3.5178033229660028E-4</v>
       </c>
       <c r="F8" s="1">
-        <v>3.0000000000000003E-4</v>
+        <v>1.5000000000000001E-4</v>
       </c>
       <c r="G8" s="5">
-        <v>3.515599741109437E-4</v>
+        <v>3.298073795208408E-4</v>
       </c>
       <c r="H8" s="1">
-        <v>3.0000000000000003E-4</v>
+        <v>1.5000000000000001E-4</v>
       </c>
       <c r="I8" s="5">
         <v>1.9402616994303117E-4</v>
@@ -2490,28 +2150,28 @@
         <v>16</v>
       </c>
       <c r="B9" s="5">
-        <v>8.0000000000000019E-3</v>
+        <v>1.9700757715135613E-3</v>
       </c>
       <c r="C9" s="5">
-        <v>7.9935696583604632E-4</v>
+        <v>1.9124982829123489E-4</v>
       </c>
       <c r="D9" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="E9" s="5">
-        <v>7.0356066459320056E-4</v>
+        <v>1.8454039930480181E-4</v>
       </c>
       <c r="F9" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="G9" s="5">
-        <v>6.596147590416816E-4</v>
+        <v>1.7883006891226079E-4</v>
       </c>
       <c r="H9" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="I9" s="5">
-        <v>3.8805233988606233E-4</v>
+        <v>9.7013084971515583E-5</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
@@ -2519,28 +2179,28 @@
         <v>17</v>
       </c>
       <c r="B10" s="5">
-        <v>1.9700757715135613E-3</v>
+        <v>3.4530390739466979E-3</v>
       </c>
       <c r="C10" s="5">
-        <v>1.9124982829123489E-4</v>
+        <v>3.3846058449864475E-4</v>
       </c>
       <c r="D10" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="E10" s="5">
-        <v>1.8454039930480181E-4</v>
+        <v>3.2294569878340315E-4</v>
       </c>
       <c r="F10" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="G10" s="5">
-        <v>1.7883006891226079E-4</v>
+        <v>3.1174237933433992E-4</v>
       </c>
       <c r="H10" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="I10" s="5">
-        <v>9.7013084971515583E-5</v>
+        <v>1.6977289870015227E-4</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -2548,115 +2208,115 @@
         <v>18</v>
       </c>
       <c r="B11" s="5">
-        <v>3.4530390739466979E-3</v>
+        <v>2.4761876858234513E-3</v>
       </c>
       <c r="C11" s="5">
-        <v>3.3846058449864475E-4</v>
+        <v>2.4121143486201491E-4</v>
       </c>
       <c r="D11" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="E11" s="5">
-        <v>3.2294569878340315E-4</v>
+        <v>2.3067549913100227E-4</v>
       </c>
       <c r="F11" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="G11" s="5">
-        <v>3.1174237933433992E-4</v>
+        <v>2.201389407504037E-4</v>
       </c>
       <c r="H11" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="I11" s="5">
-        <v>1.6977289870015227E-4</v>
+        <v>1.2126635621439448E-4</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B12" s="5">
-        <v>2.4761876858234513E-3</v>
+        <v>1.979386087282695E-3</v>
       </c>
       <c r="C12" s="5">
-        <v>2.4121143486201491E-4</v>
+        <v>1.9428853203295199E-4</v>
       </c>
       <c r="D12" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="E12" s="5">
-        <v>2.3067549913100227E-4</v>
+        <v>1.8687527039520658E-4</v>
       </c>
       <c r="F12" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="G12" s="5">
-        <v>2.201389407504037E-4</v>
+        <v>1.8253590921167207E-4</v>
       </c>
       <c r="H12" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="I12" s="5">
-        <v>1.2126635621439448E-4</v>
+        <v>9.7013084971515583E-5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B13" s="5">
-        <v>1.979386087282695E-3</v>
+        <v>2.4742326091033688E-4</v>
       </c>
       <c r="C13" s="5">
-        <v>1.9428853203295199E-4</v>
-      </c>
-      <c r="D13" s="1">
-        <v>8.0000000000000004E-4</v>
+        <v>2.4230729170731099E-5</v>
+      </c>
+      <c r="D13" s="5">
+        <v>2.3888569840924834E-4</v>
       </c>
       <c r="E13" s="5">
-        <v>1.8687527039520658E-4</v>
-      </c>
-      <c r="F13" s="1">
-        <v>3.0000000000000003E-4</v>
+        <v>2.337594436110171E-5</v>
+      </c>
+      <c r="F13" s="5">
+        <v>2.277090285662372E-4</v>
       </c>
       <c r="G13" s="5">
-        <v>1.8253590921167207E-4</v>
-      </c>
-      <c r="H13" s="1">
-        <v>3.0000000000000003E-4</v>
+        <v>2.2426571966825683E-5</v>
+      </c>
+      <c r="H13" s="5">
+        <v>2.2196037727514658E-4</v>
       </c>
       <c r="I13" s="5">
-        <v>9.7013084971515583E-5</v>
+        <v>1.2126635621439448E-5</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B14" s="5">
-        <v>2.4742326091033688E-4</v>
+        <v>1.7333313800764159E-3</v>
       </c>
       <c r="C14" s="5">
-        <v>2.4230729170731099E-5</v>
-      </c>
-      <c r="D14" s="5">
-        <v>2.3888569840924834E-4</v>
+        <v>1.703924018756886E-4</v>
+      </c>
+      <c r="D14" s="1">
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="E14" s="5">
-        <v>2.337594436110171E-5</v>
-      </c>
-      <c r="F14" s="5">
-        <v>2.277090285662372E-4</v>
+        <v>1.6091861830274718E-4</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3.0000000000000003E-4</v>
       </c>
       <c r="G14" s="5">
-        <v>2.2426571966825683E-5</v>
-      </c>
-      <c r="H14" s="5">
-        <v>2.2196037727514658E-4</v>
+        <v>1.5380748867353786E-4</v>
+      </c>
+      <c r="H14" s="1">
+        <v>3.0000000000000003E-4</v>
       </c>
       <c r="I14" s="5">
-        <v>1.2126635621439448E-5</v>
+        <v>8.4886449350076137E-5</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
@@ -2664,28 +2324,28 @@
         <v>20</v>
       </c>
       <c r="B15" s="5">
-        <v>1.7333313800764159E-3</v>
+        <v>2.9808631547078423E-3</v>
       </c>
       <c r="C15" s="5">
-        <v>1.703924018756886E-4</v>
+        <v>2.9277418149203417E-4</v>
       </c>
       <c r="D15" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="E15" s="5">
-        <v>1.6091861830274718E-4</v>
+        <v>2.7719336713683305E-4</v>
       </c>
       <c r="F15" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="G15" s="5">
-        <v>1.5380748867353786E-4</v>
+        <v>2.6268490885423374E-4</v>
       </c>
       <c r="H15" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="I15" s="5">
-        <v>8.4886449350076137E-5</v>
+        <v>1.4551962745727338E-4</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
@@ -2693,115 +2353,115 @@
         <v>21</v>
       </c>
       <c r="B16" s="5">
-        <v>2.9808631547078423E-3</v>
+        <v>3.714281528735177E-3</v>
       </c>
       <c r="C16" s="5">
-        <v>2.9277418149203417E-4</v>
+        <v>3.6346093756096649E-4</v>
       </c>
       <c r="D16" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="E16" s="5">
-        <v>2.7719336713683305E-4</v>
+        <v>3.5238999064130536E-4</v>
       </c>
       <c r="F16" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="G16" s="5">
-        <v>2.6268490885423374E-4</v>
+        <v>3.4769647827161278E-4</v>
       </c>
       <c r="H16" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="I16" s="5">
-        <v>1.4551962745727338E-4</v>
+        <v>1.8189953432159171E-4</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B17" s="5">
-        <v>4.9445639308626655E-4</v>
+        <v>9.8426814116861863E-4</v>
       </c>
       <c r="C17" s="5">
-        <v>4.8535160069751977E-5</v>
-      </c>
-      <c r="D17" s="5">
-        <v>4.7777139681849667E-4</v>
+        <v>9.6630047857710865E-5</v>
+      </c>
+      <c r="D17" s="1">
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="E17" s="5">
-        <v>4.6685815300294451E-5</v>
-      </c>
-      <c r="F17" s="5">
-        <v>4.5664824786201713E-4</v>
+        <v>9.4308381424504671E-5</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3.0000000000000003E-4</v>
       </c>
       <c r="G17" s="5">
-        <v>4.4970675219604504E-5</v>
-      </c>
-      <c r="H17" s="5">
-        <v>4.4506005352310294E-4</v>
+        <v>9.1206383510351521E-5</v>
+      </c>
+      <c r="H17" s="1">
+        <v>3.0000000000000003E-4</v>
       </c>
       <c r="I17" s="5">
-        <v>2.4253271242878896E-5</v>
+        <v>4.8506542485757792E-5</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="5">
-        <v>3.714281528735177E-3</v>
+        <v>7.4226978273101069E-4</v>
       </c>
       <c r="C18" s="5">
-        <v>3.6346093756096649E-4</v>
+        <v>7.2802740104627959E-5</v>
       </c>
       <c r="D18" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="E18" s="5">
-        <v>3.5238999064130536E-4</v>
+        <v>6.9394426605035226E-5</v>
       </c>
       <c r="F18" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="G18" s="5">
-        <v>3.4769647827161278E-4</v>
+        <v>6.7148396165000207E-5</v>
       </c>
       <c r="H18" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="I18" s="5">
-        <v>1.8189953432159171E-4</v>
+        <v>3.6379906864318345E-5</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B19" s="5">
-        <v>9.8426814116861863E-4</v>
+        <v>4.9602223988322123E-3</v>
       </c>
       <c r="C19" s="5">
-        <v>9.6630047857710865E-5</v>
+        <v>4.853516006975198E-4</v>
       </c>
       <c r="D19" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="E19" s="5">
-        <v>9.4308381424504671E-5</v>
+        <v>4.6359530436215041E-4</v>
       </c>
       <c r="F19" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="G19" s="5">
-        <v>9.1206383510351521E-5</v>
+        <v>4.4279019720409331E-4</v>
       </c>
       <c r="H19" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="I19" s="5">
-        <v>4.8506542485757792E-5</v>
+        <v>2.4253271242878895E-4</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -2809,354 +2469,159 @@
         <v>24</v>
       </c>
       <c r="B20" s="5">
-        <v>7.4226978273101069E-4</v>
+        <v>1.9840889595328847E-3</v>
       </c>
       <c r="C20" s="5">
-        <v>7.2802740104627959E-5</v>
+        <v>1.9414064027900791E-4</v>
       </c>
       <c r="D20" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="E20" s="5">
-        <v>6.9394426605035226E-5</v>
+        <v>1.8543812174486016E-4</v>
       </c>
       <c r="F20" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="G20" s="5">
-        <v>6.7148396165000207E-5</v>
+        <v>1.7711607888163734E-4</v>
       </c>
       <c r="H20" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="I20" s="5">
-        <v>3.6379906864318345E-5</v>
+        <v>9.7013084971515583E-5</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>25</v>
+      <c r="A21" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B21" s="5">
-        <v>4.9602223988322119E-4</v>
+        <v>2.4761876858234513E-4</v>
       </c>
       <c r="C21" s="5">
-        <v>4.8535160069751977E-5</v>
+        <v>2.4341771696526945E-5</v>
       </c>
       <c r="D21" s="5">
-        <v>4.7566823169218855E-4</v>
+        <v>2.3906228536404344E-4</v>
       </c>
       <c r="E21" s="5">
-        <v>4.635953043621504E-5</v>
+        <v>2.3543216837781408E-5</v>
       </c>
       <c r="F21" s="5">
-        <v>4.5268585116385211E-4</v>
+        <v>2.334290765014721E-4</v>
       </c>
       <c r="G21" s="5">
-        <v>4.4279019720409334E-5</v>
+        <v>2.2832412393100853E-5</v>
       </c>
       <c r="H21" s="5">
-        <v>4.3325564085736328E-4</v>
+        <v>2.2210237788307778E-4</v>
       </c>
       <c r="I21" s="5">
-        <v>2.4253271242878896E-5</v>
+        <v>1.2126635621439448E-5</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>26</v>
+      <c r="A22" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B22" s="5">
-        <v>4.9602223988322123E-3</v>
+        <v>9.9125888433051895E-3</v>
       </c>
       <c r="C22" s="5">
-        <v>4.853516006975198E-4</v>
+        <v>9.6776160685979259E-4</v>
       </c>
       <c r="D22" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="E22" s="5">
-        <v>4.6359530436215041E-4</v>
+        <v>9.3437635197603295E-4</v>
       </c>
       <c r="F22" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="G22" s="5">
-        <v>4.4279019720409331E-4</v>
+        <v>9.0961330323741367E-4</v>
       </c>
       <c r="H22" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="I22" s="5">
-        <v>2.4253271242878895E-4</v>
+        <v>4.850654248575779E-4</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>27</v>
+      <c r="A23" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B23" s="5">
-        <v>1.9840889595328847E-3</v>
+        <v>1.2265080218123586E-3</v>
       </c>
       <c r="C23" s="5">
-        <v>1.9414064027900791E-4</v>
+        <v>1.2024440754700463E-4</v>
       </c>
       <c r="D23" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="E23" s="5">
-        <v>1.8543812174486016E-4</v>
+        <v>1.1324675411436813E-4</v>
       </c>
       <c r="F23" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="G23" s="5">
-        <v>1.7711607888163734E-4</v>
+        <v>1.1000034653859286E-4</v>
       </c>
       <c r="H23" s="1">
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="I23" s="5">
-        <v>9.7013084971515583E-5</v>
+        <v>6.0633178107197238E-5</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B24" s="5">
-        <v>2.4761876858234513E-4</v>
+        <v>1.2380938429117257E-3</v>
       </c>
       <c r="C24" s="5">
-        <v>2.4341771696526945E-5</v>
-      </c>
-      <c r="D24" s="5">
-        <v>2.3906228536404344E-4</v>
+        <v>1.2078755982213858E-4</v>
+      </c>
+      <c r="D24" s="1">
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="E24" s="5">
-        <v>2.3543216837781408E-5</v>
-      </c>
-      <c r="F24" s="5">
-        <v>2.334290765014721E-4</v>
+        <v>1.1606062195794044E-4</v>
+      </c>
+      <c r="F24" s="1">
+        <v>3.0000000000000003E-4</v>
       </c>
       <c r="G24" s="5">
-        <v>2.2832412393100853E-5</v>
-      </c>
-      <c r="H24" s="5">
-        <v>2.2210237788307778E-4</v>
+        <v>1.1370166290467671E-4</v>
+      </c>
+      <c r="H24" s="1">
+        <v>3.0000000000000003E-4</v>
       </c>
       <c r="I24" s="5">
-        <v>1.2126635621439448E-5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="5">
-        <v>9.9125888433051895E-3</v>
-      </c>
-      <c r="C25" s="5">
-        <v>9.6776160685979259E-4</v>
-      </c>
-      <c r="D25" s="1">
-        <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="E25" s="5">
-        <v>9.3437635197603295E-4</v>
-      </c>
-      <c r="F25" s="1">
-        <v>3.0000000000000003E-4</v>
-      </c>
-      <c r="G25" s="5">
-        <v>9.0961330323741367E-4</v>
-      </c>
-      <c r="H25" s="1">
-        <v>3.0000000000000003E-4</v>
-      </c>
-      <c r="I25" s="5">
-        <v>4.850654248575779E-4</v>
+        <v>6.0633178107197238E-5</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="5">
-        <v>5.0000000000000012E-4</v>
-      </c>
-      <c r="C26" s="5">
-        <v>5.0000000000000043E-5</v>
-      </c>
-      <c r="D26" s="5">
-        <v>5.0000000000000012E-4</v>
-      </c>
-      <c r="E26" s="5">
-        <v>5.0000000000000043E-5</v>
-      </c>
-      <c r="F26" s="5">
-        <v>5.0000000000000012E-4</v>
-      </c>
-      <c r="G26" s="5">
-        <v>5.0000000000000043E-5</v>
-      </c>
-      <c r="H26" s="5">
-        <v>5.0000000000000012E-4</v>
-      </c>
-      <c r="I26" s="5">
-        <v>5.0000000000000043E-5</v>
-      </c>
+      <c r="A26" s="3"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="5">
-        <v>5.0000000000000012E-4</v>
-      </c>
-      <c r="C27" s="5">
-        <v>5.0000000000000043E-5</v>
-      </c>
-      <c r="D27" s="5">
-        <v>5.0000000000000012E-4</v>
-      </c>
-      <c r="E27" s="5">
-        <v>5.0000000000000043E-5</v>
-      </c>
-      <c r="F27" s="5">
-        <v>5.0000000000000012E-4</v>
-      </c>
-      <c r="G27" s="5">
-        <v>5.0000000000000043E-5</v>
-      </c>
-      <c r="H27" s="5">
-        <v>5.0000000000000012E-4</v>
-      </c>
-      <c r="I27" s="5">
-        <v>5.0000000000000043E-5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="5">
-        <v>5.0000000000000012E-4</v>
-      </c>
-      <c r="C28" s="5">
-        <v>5.0000000000000043E-5</v>
-      </c>
-      <c r="D28" s="5">
-        <v>5.0000000000000012E-4</v>
-      </c>
-      <c r="E28" s="5">
-        <v>5.0000000000000043E-5</v>
-      </c>
-      <c r="F28" s="5">
-        <v>5.0000000000000012E-4</v>
-      </c>
-      <c r="G28" s="5">
-        <v>5.0000000000000043E-5</v>
-      </c>
-      <c r="H28" s="5">
-        <v>5.0000000000000012E-4</v>
-      </c>
-      <c r="I28" s="5">
-        <v>5.0000000000000043E-5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="5">
-        <v>5.0000000000000012E-4</v>
-      </c>
-      <c r="C29" s="5">
-        <v>4.9959810364752895E-5</v>
-      </c>
-      <c r="D29" s="5">
-        <v>4.7706732717378721E-4</v>
-      </c>
-      <c r="E29" s="5">
-        <v>4.3972541537075035E-5</v>
-      </c>
-      <c r="F29" s="5">
-        <v>4.2162645838521675E-4</v>
-      </c>
-      <c r="G29" s="5">
-        <v>4.12259224401051E-5</v>
-      </c>
-      <c r="H29" s="5">
-        <v>4.1023928592577352E-4</v>
-      </c>
-      <c r="I29" s="5">
-        <v>2.4253271242878896E-5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="5">
-        <v>1.2265080218123586E-3</v>
-      </c>
-      <c r="C30" s="5">
-        <v>1.2024440754700463E-4</v>
-      </c>
-      <c r="D30" s="1">
-        <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="E30" s="5">
-        <v>1.1324675411436813E-4</v>
-      </c>
-      <c r="F30" s="1">
-        <v>3.0000000000000003E-4</v>
-      </c>
-      <c r="G30" s="5">
-        <v>1.1000034653859286E-4</v>
-      </c>
-      <c r="H30" s="1">
-        <v>3.0000000000000003E-4</v>
-      </c>
-      <c r="I30" s="5">
-        <v>6.0633178107197238E-5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="5">
-        <v>1.2380938429117257E-3</v>
-      </c>
-      <c r="C31" s="5">
-        <v>1.2078755982213858E-4</v>
-      </c>
-      <c r="D31" s="1">
-        <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="E31" s="5">
-        <v>1.1606062195794044E-4</v>
-      </c>
-      <c r="F31" s="1">
-        <v>3.0000000000000003E-4</v>
-      </c>
-      <c r="G31" s="5">
-        <v>1.1370166290467671E-4</v>
-      </c>
-      <c r="H31" s="1">
-        <v>3.0000000000000003E-4</v>
-      </c>
-      <c r="I31" s="5">
-        <v>6.0633178107197238E-5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="3"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="3"/>
+      <c r="A27" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3166,10 +2631,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3244,32 +2709,32 @@
         <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>1.2371163045516843E-5</v>
+        <v>2.4801111994161059E-4</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:E31" si="0">B3/10</f>
-        <v>1.2371163045516842E-6</v>
+        <f t="shared" ref="C3:C24" si="0">B3/10</f>
+        <v>2.4801111994161058E-5</v>
       </c>
       <c r="D3" s="1">
-        <v>1.1935474578123703E-5</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3" si="1">D3/10</f>
-        <v>1.1935474578123704E-6</v>
+        <v>4.0000000000000007E-6</v>
       </c>
       <c r="F3" s="1">
-        <v>1.1408494325729498E-5</v>
+        <v>1.5000000000000002E-5</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3" si="2">F3/10</f>
-        <v>1.1408494325729497E-6</v>
+        <v>1.5000000000000002E-6</v>
       </c>
       <c r="H3" s="1">
-        <v>1.1105118894153889E-5</v>
+        <v>1.5000000000000002E-5</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3" si="3">H3/10</f>
-        <v>1.1105118894153888E-6</v>
+        <v>1.5000000000000002E-6</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -3277,11 +2742,11 @@
         <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>2.4801111994161059E-4</v>
+        <v>2.4683939166376463E-4</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>2.4801111994161058E-5</v>
+        <v>2.4683939166376464E-5</v>
       </c>
       <c r="D4" s="1">
         <v>4.0000000000000003E-5</v>
@@ -3310,32 +2775,32 @@
         <v>12</v>
       </c>
       <c r="B5" s="1">
-        <v>2.4683939166376463E-4</v>
+        <v>1.0895225817623185E-4</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
-        <v>2.4683939166376464E-5</v>
+        <v>1.0895225817623186E-5</v>
       </c>
       <c r="D5" s="1">
-        <v>4.0000000000000003E-5</v>
+        <v>7.9999999999999996E-6</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" ref="E5" si="7">D5/10</f>
-        <v>4.0000000000000007E-6</v>
+        <v>7.9999999999999996E-7</v>
       </c>
       <c r="F5" s="1">
-        <v>1.5000000000000002E-5</v>
+        <v>3.0000000000000001E-6</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" ref="G5" si="8">F5/10</f>
-        <v>1.5000000000000002E-6</v>
+        <v>2.9999999999999999E-7</v>
       </c>
       <c r="H5" s="1">
-        <v>1.5000000000000002E-5</v>
+        <v>3.0000000000000001E-6</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ref="I5" si="9">H5/10</f>
-        <v>1.5000000000000002E-6</v>
+        <v>2.9999999999999999E-7</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -3343,32 +2808,32 @@
         <v>13</v>
       </c>
       <c r="B6" s="1">
-        <v>1.0895225817623185E-4</v>
+        <v>1.2312973571959758E-4</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
-        <v>1.0895225817623186E-5</v>
+        <v>1.2312973571959758E-5</v>
       </c>
       <c r="D6" s="1">
-        <v>7.9999999999999996E-6</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" ref="E6" si="10">D6/10</f>
-        <v>7.9999999999999996E-7</v>
+        <v>4.0000000000000007E-6</v>
       </c>
       <c r="F6" s="1">
-        <v>3.0000000000000001E-6</v>
+        <v>1.5000000000000002E-5</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" ref="G6" si="11">F6/10</f>
-        <v>2.9999999999999999E-7</v>
+        <v>1.5000000000000002E-6</v>
       </c>
       <c r="H6" s="1">
-        <v>3.0000000000000001E-6</v>
+        <v>1.5000000000000002E-5</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" ref="I6" si="12">H6/10</f>
-        <v>2.9999999999999999E-7</v>
+        <v>1.5000000000000002E-6</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -3376,32 +2841,32 @@
         <v>14</v>
       </c>
       <c r="B7" s="1">
-        <v>1.2312973571959758E-4</v>
+        <v>3.9587721745653903E-5</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
-        <v>1.2312973571959758E-5</v>
+        <v>3.9587721745653904E-6</v>
       </c>
       <c r="D7" s="1">
-        <v>4.0000000000000003E-5</v>
+        <v>7.9999999999999996E-6</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" ref="E7" si="13">D7/10</f>
-        <v>4.0000000000000007E-6</v>
+        <v>7.9999999999999996E-7</v>
       </c>
       <c r="F7" s="1">
-        <v>1.5000000000000002E-5</v>
+        <v>3.0000000000000001E-6</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" ref="G7" si="14">F7/10</f>
-        <v>1.5000000000000002E-6</v>
+        <v>2.9999999999999999E-7</v>
       </c>
       <c r="H7" s="1">
-        <v>1.5000000000000002E-5</v>
+        <v>3.0000000000000001E-6</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" ref="I7" si="15">H7/10</f>
-        <v>1.5000000000000002E-6</v>
+        <v>2.9999999999999999E-7</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -3409,32 +2874,32 @@
         <v>15</v>
       </c>
       <c r="B8" s="1">
-        <v>3.9587721745653903E-5</v>
+        <v>5.3333333333333347E-5</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
-        <v>3.9587721745653904E-6</v>
+        <v>5.3333333333333345E-6</v>
       </c>
       <c r="D8" s="1">
-        <v>7.9999999999999996E-6</v>
+        <v>5.3333333333333337E-6</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" ref="E8" si="16">D8/10</f>
-        <v>7.9999999999999996E-7</v>
+        <v>5.3333333333333334E-7</v>
       </c>
       <c r="F8" s="1">
-        <v>3.0000000000000001E-6</v>
+        <v>2.0000000000000003E-6</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" ref="G8" si="17">F8/10</f>
-        <v>2.9999999999999999E-7</v>
+        <v>2.0000000000000004E-7</v>
       </c>
       <c r="H8" s="1">
-        <v>3.0000000000000001E-6</v>
+        <v>2.0000000000000003E-6</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" ref="I8" si="18">H8/10</f>
-        <v>2.9999999999999999E-7</v>
+        <v>2.0000000000000004E-7</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -3442,32 +2907,32 @@
         <v>16</v>
       </c>
       <c r="B9" s="1">
-        <v>5.3333333333333347E-5</v>
+        <v>1.9700757715135613E-4</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
-        <v>5.3333333333333345E-6</v>
+        <v>1.9700757715135615E-5</v>
       </c>
       <c r="D9" s="1">
-        <v>5.3333333333333337E-6</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" ref="E9" si="19">D9/10</f>
-        <v>5.3333333333333334E-7</v>
+        <v>4.0000000000000007E-6</v>
       </c>
       <c r="F9" s="1">
-        <v>2.0000000000000003E-6</v>
+        <v>1.5000000000000002E-5</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" ref="G9" si="20">F9/10</f>
-        <v>2.0000000000000004E-7</v>
+        <v>1.5000000000000002E-6</v>
       </c>
       <c r="H9" s="1">
-        <v>2.0000000000000003E-6</v>
+        <v>1.5000000000000002E-5</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" ref="I9" si="21">H9/10</f>
-        <v>2.0000000000000004E-7</v>
+        <v>1.5000000000000002E-6</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -3475,32 +2940,32 @@
         <v>17</v>
       </c>
       <c r="B10" s="1">
-        <v>1.9700757715135613E-4</v>
+        <v>2.4664564813904984E-4</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
-        <v>1.9700757715135615E-5</v>
+        <v>2.4664564813904983E-5</v>
       </c>
       <c r="D10" s="1">
-        <v>4.0000000000000003E-5</v>
+        <v>2.6666666666666667E-5</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" ref="E10" si="22">D10/10</f>
-        <v>4.0000000000000007E-6</v>
+        <v>2.6666666666666668E-6</v>
       </c>
       <c r="F10" s="1">
-        <v>1.5000000000000002E-5</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" ref="G10" si="23">F10/10</f>
-        <v>1.5000000000000002E-6</v>
+        <v>1.0000000000000002E-6</v>
       </c>
       <c r="H10" s="1">
-        <v>1.5000000000000002E-5</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" ref="I10" si="24">H10/10</f>
-        <v>1.5000000000000002E-6</v>
+        <v>1.0000000000000002E-6</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -3508,131 +2973,131 @@
         <v>18</v>
       </c>
       <c r="B11" s="1">
-        <v>2.4664564813904984E-4</v>
+        <v>1.2380938429117257E-4</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="0"/>
-        <v>2.4664564813904983E-5</v>
+        <v>1.2380938429117256E-5</v>
       </c>
       <c r="D11" s="1">
-        <v>2.6666666666666667E-5</v>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" ref="E11" si="25">D11/10</f>
-        <v>2.6666666666666668E-6</v>
+        <v>2.0000000000000003E-6</v>
       </c>
       <c r="F11" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>7.500000000000001E-6</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" ref="G11" si="26">F11/10</f>
-        <v>1.0000000000000002E-6</v>
+        <v>7.5000000000000012E-7</v>
       </c>
       <c r="H11" s="1">
-        <v>1.0000000000000001E-5</v>
+        <v>7.500000000000001E-6</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" ref="I11" si="27">H11/10</f>
-        <v>1.0000000000000002E-6</v>
+        <v>7.5000000000000012E-7</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1">
-        <v>1.2380938429117257E-4</v>
+        <v>1.9793860872826951E-5</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="0"/>
-        <v>1.2380938429117256E-5</v>
+        <v>1.9793860872826952E-6</v>
       </c>
       <c r="D12" s="1">
-        <v>2.0000000000000002E-5</v>
+        <v>7.9999999999999996E-6</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" ref="E12" si="28">D12/10</f>
-        <v>2.0000000000000003E-6</v>
+        <v>7.9999999999999996E-7</v>
       </c>
       <c r="F12" s="1">
-        <v>7.500000000000001E-6</v>
+        <v>3.0000000000000001E-6</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" ref="G12" si="29">F12/10</f>
-        <v>7.5000000000000012E-7</v>
+        <v>2.9999999999999999E-7</v>
       </c>
       <c r="H12" s="1">
-        <v>7.500000000000001E-6</v>
+        <v>3.0000000000000001E-6</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" ref="I12" si="30">H12/10</f>
-        <v>7.5000000000000012E-7</v>
+        <v>2.9999999999999999E-7</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1">
-        <v>1.9793860872826951E-5</v>
+        <v>2.4742326091033689E-6</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" si="0"/>
-        <v>1.9793860872826952E-6</v>
+        <v>2.474232609103369E-7</v>
       </c>
       <c r="D13" s="1">
-        <v>7.9999999999999996E-6</v>
+        <v>2.3888569840924832E-6</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" ref="E13" si="31">D13/10</f>
-        <v>7.9999999999999996E-7</v>
+        <v>2.3888569840924831E-7</v>
       </c>
       <c r="F13" s="1">
-        <v>3.0000000000000001E-6</v>
+        <v>2.2770902856623721E-6</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" ref="G13" si="32">F13/10</f>
-        <v>2.9999999999999999E-7</v>
+        <v>2.2770902856623722E-7</v>
       </c>
       <c r="H13" s="1">
-        <v>3.0000000000000001E-6</v>
+        <v>2.2196037727514661E-6</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" ref="I13" si="33">H13/10</f>
-        <v>2.9999999999999999E-7</v>
+        <v>2.2196037727514661E-7</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1">
-        <v>2.4742326091033689E-6</v>
+        <v>8.6666569003820799E-5</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="0"/>
-        <v>2.474232609103369E-7</v>
+        <v>8.6666569003820799E-6</v>
       </c>
       <c r="D14" s="1">
-        <v>2.3888569840924832E-6</v>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" ref="E14" si="34">D14/10</f>
-        <v>2.3888569840924831E-7</v>
+        <v>2.0000000000000003E-6</v>
       </c>
       <c r="F14" s="1">
-        <v>2.2770902856623721E-6</v>
+        <v>7.500000000000001E-6</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" ref="G14" si="35">F14/10</f>
-        <v>2.2770902856623722E-7</v>
+        <v>7.5000000000000012E-7</v>
       </c>
       <c r="H14" s="1">
-        <v>2.2196037727514661E-6</v>
+        <v>7.500000000000001E-6</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" ref="I14" si="36">H14/10</f>
-        <v>2.2196037727514661E-7</v>
+        <v>7.5000000000000012E-7</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -3640,11 +3105,11 @@
         <v>20</v>
       </c>
       <c r="B15" s="1">
-        <v>8.6666569003820799E-5</v>
+        <v>1.4904315773539212E-4</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="0"/>
-        <v>8.6666569003820799E-6</v>
+        <v>1.4904315773539212E-5</v>
       </c>
       <c r="D15" s="1">
         <v>2.0000000000000002E-5</v>
@@ -3673,11 +3138,11 @@
         <v>21</v>
       </c>
       <c r="B16" s="1">
-        <v>1.4904315773539212E-4</v>
+        <v>1.8571407643675885E-4</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="0"/>
-        <v>1.4904315773539212E-5</v>
+        <v>1.8571407643675884E-5</v>
       </c>
       <c r="D16" s="1">
         <v>2.0000000000000002E-5</v>
@@ -3703,80 +3168,80 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1">
-        <v>1.2361409827156663E-5</v>
+        <v>9.8426814116861865E-5</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" si="0"/>
-        <v>1.2361409827156663E-6</v>
+        <v>9.8426814116861859E-6</v>
       </c>
       <c r="D17" s="1">
-        <v>1.1944284920462416E-5</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" ref="E17" si="43">D17/10</f>
-        <v>1.1944284920462416E-6</v>
+        <v>4.0000000000000007E-6</v>
       </c>
       <c r="F17" s="1">
-        <v>1.1416206196550428E-5</v>
+        <v>1.5000000000000002E-5</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" ref="G17" si="44">F17/10</f>
-        <v>1.1416206196550429E-6</v>
+        <v>1.5000000000000002E-6</v>
       </c>
       <c r="H17" s="1">
-        <v>1.1126501338077573E-5</v>
+        <v>1.5000000000000002E-5</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" ref="I17" si="45">H17/10</f>
-        <v>1.1126501338077573E-6</v>
+        <v>1.5000000000000002E-6</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1">
-        <v>1.8571407643675885E-4</v>
+        <v>7.4226978273101067E-5</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" si="0"/>
-        <v>1.8571407643675884E-5</v>
+        <v>7.4226978273101063E-6</v>
       </c>
       <c r="D18" s="1">
-        <v>2.0000000000000002E-5</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="E18" s="1">
         <f t="shared" ref="E18" si="46">D18/10</f>
-        <v>2.0000000000000003E-6</v>
+        <v>4.0000000000000007E-6</v>
       </c>
       <c r="F18" s="1">
-        <v>7.500000000000001E-6</v>
+        <v>1.5000000000000002E-5</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" ref="G18" si="47">F18/10</f>
-        <v>7.5000000000000012E-7</v>
+        <v>1.5000000000000002E-6</v>
       </c>
       <c r="H18" s="1">
-        <v>7.500000000000001E-6</v>
+        <v>1.5000000000000002E-5</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" ref="I18" si="48">H18/10</f>
-        <v>7.5000000000000012E-7</v>
+        <v>1.5000000000000002E-6</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1">
-        <v>9.8426814116861865E-5</v>
+        <v>4.9602223988322119E-4</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" si="0"/>
-        <v>9.8426814116861859E-6</v>
+        <v>4.9602223988322116E-5</v>
       </c>
       <c r="D19" s="1">
         <v>4.0000000000000003E-5</v>
@@ -3805,77 +3270,77 @@
         <v>24</v>
       </c>
       <c r="B20" s="1">
-        <v>7.4226978273101067E-5</v>
+        <v>1.3227259730219232E-5</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" si="0"/>
-        <v>7.4226978273101063E-6</v>
+        <v>1.3227259730219233E-6</v>
       </c>
       <c r="D20" s="1">
-        <v>4.0000000000000003E-5</v>
+        <v>5.3333333333333337E-6</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" ref="E20" si="52">D20/10</f>
-        <v>4.0000000000000007E-6</v>
+        <v>5.3333333333333334E-7</v>
       </c>
       <c r="F20" s="1">
-        <v>1.5000000000000002E-5</v>
+        <v>2.0000000000000003E-6</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" ref="G20" si="53">F20/10</f>
-        <v>1.5000000000000002E-6</v>
+        <v>2.0000000000000004E-7</v>
       </c>
       <c r="H20" s="1">
-        <v>1.5000000000000002E-5</v>
+        <v>2.0000000000000003E-6</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" ref="I20" si="54">H20/10</f>
-        <v>1.5000000000000002E-6</v>
+        <v>2.0000000000000004E-7</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>25</v>
+      <c r="A21" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B21" s="1">
-        <v>1.2400555997080529E-5</v>
+        <v>1.2380938429117256E-5</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" si="0"/>
-        <v>1.2400555997080528E-6</v>
+        <v>1.2380938429117257E-6</v>
       </c>
       <c r="D21" s="1">
-        <v>1.1891705792304714E-5</v>
+        <v>1.1953114268202172E-5</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" ref="E21" si="55">D21/10</f>
-        <v>1.1891705792304714E-6</v>
+        <v>1.1953114268202171E-6</v>
       </c>
       <c r="F21" s="1">
-        <v>1.1317146279096302E-5</v>
+        <v>1.1671453825073604E-5</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" ref="G21" si="56">F21/10</f>
-        <v>1.1317146279096303E-6</v>
+        <v>1.1671453825073603E-6</v>
       </c>
       <c r="H21" s="1">
-        <v>1.0831391021434082E-5</v>
+        <v>1.1105118894153889E-5</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" ref="I21" si="57">H21/10</f>
-        <v>1.0831391021434082E-6</v>
+        <v>1.1105118894153888E-6</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>26</v>
+      <c r="A22" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B22" s="1">
-        <v>4.9602223988322119E-4</v>
+        <v>4.9562944216525952E-4</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" si="0"/>
-        <v>4.9602223988322116E-5</v>
+        <v>4.9562944216525955E-5</v>
       </c>
       <c r="D22" s="1">
         <v>4.0000000000000003E-5</v>
@@ -3898,317 +3363,89 @@
         <f t="shared" ref="I22" si="60">H22/10</f>
         <v>1.5000000000000002E-6</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>27</v>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B23" s="1">
-        <v>1.3227259730219232E-5</v>
+        <v>2.4530160436247174E-5</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" si="0"/>
-        <v>1.3227259730219233E-6</v>
+        <v>2.4530160436247172E-6</v>
       </c>
       <c r="D23" s="1">
-        <v>5.3333333333333337E-6</v>
+        <v>7.9999999999999996E-6</v>
       </c>
       <c r="E23" s="1">
         <f t="shared" ref="E23" si="61">D23/10</f>
-        <v>5.3333333333333334E-7</v>
+        <v>7.9999999999999996E-7</v>
       </c>
       <c r="F23" s="1">
-        <v>2.0000000000000003E-6</v>
+        <v>3.0000000000000001E-6</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" ref="G23" si="62">F23/10</f>
-        <v>2.0000000000000004E-7</v>
+        <v>2.9999999999999999E-7</v>
       </c>
       <c r="H23" s="1">
-        <v>2.0000000000000003E-6</v>
+        <v>3.0000000000000001E-6</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" ref="I23" si="63">H23/10</f>
-        <v>2.0000000000000004E-7</v>
+        <v>2.9999999999999999E-7</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1">
-        <v>1.2380938429117256E-5</v>
+        <v>2.4761876858234513E-5</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" si="0"/>
-        <v>1.2380938429117257E-6</v>
+        <v>2.4761876858234514E-6</v>
       </c>
       <c r="D24" s="1">
-        <v>1.1953114268202172E-5</v>
+        <v>7.9999999999999996E-6</v>
       </c>
       <c r="E24" s="1">
         <f t="shared" ref="E24" si="64">D24/10</f>
-        <v>1.1953114268202171E-6</v>
+        <v>7.9999999999999996E-7</v>
       </c>
       <c r="F24" s="1">
-        <v>1.1671453825073604E-5</v>
+        <v>3.0000000000000001E-6</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" ref="G24" si="65">F24/10</f>
-        <v>1.1671453825073603E-6</v>
+        <v>2.9999999999999999E-7</v>
       </c>
       <c r="H24" s="1">
-        <v>1.1105118894153889E-5</v>
+        <v>3.0000000000000001E-6</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" ref="I24" si="66">H24/10</f>
-        <v>1.1105118894153888E-6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="1">
-        <v>4.9562944216525952E-4</v>
-      </c>
-      <c r="C25" s="1">
-        <f t="shared" si="0"/>
-        <v>4.9562944216525955E-5</v>
-      </c>
-      <c r="D25" s="1">
-        <v>4.0000000000000003E-5</v>
-      </c>
-      <c r="E25" s="1">
-        <f t="shared" ref="E25" si="67">D25/10</f>
-        <v>4.0000000000000007E-6</v>
-      </c>
-      <c r="F25" s="1">
-        <v>1.5000000000000002E-5</v>
-      </c>
-      <c r="G25" s="1">
-        <f t="shared" ref="G25" si="68">F25/10</f>
-        <v>1.5000000000000002E-6</v>
-      </c>
-      <c r="H25" s="1">
-        <v>1.5000000000000002E-5</v>
-      </c>
-      <c r="I25" s="1">
-        <f t="shared" ref="I25" si="69">H25/10</f>
-        <v>1.5000000000000002E-6</v>
-      </c>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
+        <v>2.9999999999999999E-7</v>
+      </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="1">
-        <v>1.2500000000000002E-5</v>
-      </c>
-      <c r="C26" s="1">
-        <f t="shared" si="0"/>
-        <v>1.2500000000000003E-6</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1.2500000000000002E-5</v>
-      </c>
-      <c r="E26" s="1">
-        <f t="shared" ref="E26" si="70">D26/10</f>
-        <v>1.2500000000000003E-6</v>
-      </c>
-      <c r="F26" s="1">
-        <v>1.2500000000000002E-5</v>
-      </c>
-      <c r="G26" s="1">
-        <f t="shared" ref="G26" si="71">F26/10</f>
-        <v>1.2500000000000003E-6</v>
-      </c>
-      <c r="H26" s="1">
-        <v>1.2500000000000002E-5</v>
-      </c>
-      <c r="I26" s="1">
-        <f t="shared" ref="I26" si="72">H26/10</f>
-        <v>1.2500000000000003E-6</v>
-      </c>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="1">
-        <v>1.2500000000000002E-5</v>
-      </c>
-      <c r="C27" s="1">
-        <f t="shared" si="0"/>
-        <v>1.2500000000000003E-6</v>
-      </c>
-      <c r="D27" s="1">
-        <v>1.2500000000000002E-5</v>
-      </c>
-      <c r="E27" s="1">
-        <f t="shared" ref="E27" si="73">D27/10</f>
-        <v>1.2500000000000003E-6</v>
-      </c>
-      <c r="F27" s="1">
-        <v>1.2500000000000002E-5</v>
-      </c>
-      <c r="G27" s="1">
-        <f t="shared" ref="G27" si="74">F27/10</f>
-        <v>1.2500000000000003E-6</v>
-      </c>
-      <c r="H27" s="1">
-        <v>1.2500000000000002E-5</v>
-      </c>
-      <c r="I27" s="1">
-        <f t="shared" ref="I27" si="75">H27/10</f>
-        <v>1.2500000000000003E-6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="1">
-        <v>1.2500000000000002E-5</v>
-      </c>
-      <c r="C28" s="1">
-        <f t="shared" si="0"/>
-        <v>1.2500000000000003E-6</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1.2500000000000002E-5</v>
-      </c>
-      <c r="E28" s="1">
-        <f t="shared" ref="E28" si="76">D28/10</f>
-        <v>1.2500000000000003E-6</v>
-      </c>
-      <c r="F28" s="1">
-        <v>1.2500000000000002E-5</v>
-      </c>
-      <c r="G28" s="1">
-        <f t="shared" ref="G28" si="77">F28/10</f>
-        <v>1.2500000000000003E-6</v>
-      </c>
-      <c r="H28" s="1">
-        <v>1.2500000000000002E-5</v>
-      </c>
-      <c r="I28" s="1">
-        <f t="shared" ref="I28" si="78">H28/10</f>
-        <v>1.2500000000000003E-6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1">
-        <v>1.2500000000000002E-5</v>
-      </c>
-      <c r="C29" s="1">
-        <f t="shared" si="0"/>
-        <v>1.2500000000000003E-6</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1.192668317934468E-5</v>
-      </c>
-      <c r="E29" s="1">
-        <f t="shared" ref="E29" si="79">D29/10</f>
-        <v>1.1926683179344681E-6</v>
-      </c>
-      <c r="F29" s="1">
-        <v>1.0540661459630418E-5</v>
-      </c>
-      <c r="G29" s="1">
-        <f t="shared" ref="G29" si="80">F29/10</f>
-        <v>1.0540661459630418E-6</v>
-      </c>
-      <c r="H29" s="1">
-        <v>1.0255982148144338E-5</v>
-      </c>
-      <c r="I29" s="1">
-        <f t="shared" ref="I29" si="81">H29/10</f>
-        <v>1.0255982148144339E-6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1">
-        <v>2.4530160436247174E-5</v>
-      </c>
-      <c r="C30" s="1">
-        <f t="shared" si="0"/>
-        <v>2.4530160436247172E-6</v>
-      </c>
-      <c r="D30" s="1">
-        <v>7.9999999999999996E-6</v>
-      </c>
-      <c r="E30" s="1">
-        <f t="shared" ref="E30" si="82">D30/10</f>
-        <v>7.9999999999999996E-7</v>
-      </c>
-      <c r="F30" s="1">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="G30" s="1">
-        <f t="shared" ref="G30" si="83">F30/10</f>
-        <v>2.9999999999999999E-7</v>
-      </c>
-      <c r="H30" s="1">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="I30" s="1">
-        <f t="shared" ref="I30" si="84">H30/10</f>
-        <v>2.9999999999999999E-7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1">
-        <v>2.4761876858234513E-5</v>
-      </c>
-      <c r="C31" s="1">
-        <f t="shared" si="0"/>
-        <v>2.4761876858234514E-6</v>
-      </c>
-      <c r="D31" s="1">
-        <v>7.9999999999999996E-6</v>
-      </c>
-      <c r="E31" s="1">
-        <f t="shared" ref="E31" si="85">D31/10</f>
-        <v>7.9999999999999996E-7</v>
-      </c>
-      <c r="F31" s="1">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="G31" s="1">
-        <f t="shared" ref="G31" si="86">F31/10</f>
-        <v>2.9999999999999999E-7</v>
-      </c>
-      <c r="H31" s="1">
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="I31" s="1">
-        <f t="shared" ref="I31" si="87">H31/10</f>
-        <v>2.9999999999999999E-7</v>
-      </c>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>